<commit_message>
starting to build envi from read_fram functions, added lu_stock sheet, and demo abundance calcs
</commit_message>
<xml_diff>
--- a/StaticTables.xlsx
+++ b/StaticTables.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stateofwa-my.sharepoint.com/personal/daniel_auerbach_dfw_wa_gov/Documents/code/PeriodicReport/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{793868AE-9DA0-439D-B941-FC5A2F22A4BB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{A43A8261-80A6-4E47-B9A6-77FA729BAE80}"/>
+  <xr:revisionPtr revIDLastSave="44" documentId="13_ncr:1_{793868AE-9DA0-439D-B941-FC5A2F22A4BB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{E2757023-91D6-413D-8147-473D2925A4D1}"/>
   <bookViews>
-    <workbookView xWindow="216" yWindow="144" windowWidth="22032" windowHeight="12180" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="924" yWindow="324" windowWidth="19872" windowHeight="11712" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="members" sheetId="5" r:id="rId1"/>
-    <sheet name="RunFiles" sheetId="1" r:id="rId2"/>
-    <sheet name="CUs" sheetId="2" r:id="rId3"/>
-    <sheet name="Acronyms" sheetId="3" r:id="rId4"/>
+    <sheet name="lu_stock" sheetId="6" r:id="rId2"/>
+    <sheet name="RunFiles" sheetId="1" r:id="rId3"/>
+    <sheet name="CUs" sheetId="2" r:id="rId4"/>
+    <sheet name="Acronyms" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="190">
   <si>
     <t>BK04.Cmd</t>
   </si>
@@ -502,6 +503,102 @@
   </si>
   <si>
     <t>Lower Fraser Fishery Alliance</t>
+  </si>
+  <si>
+    <t>PSCStock</t>
+  </si>
+  <si>
+    <t>Skagit</t>
+  </si>
+  <si>
+    <t>imu</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>US Inside</t>
+  </si>
+  <si>
+    <t>Stillaguamish</t>
+  </si>
+  <si>
+    <t>Snohomish</t>
+  </si>
+  <si>
+    <t>Hood Canal</t>
+  </si>
+  <si>
+    <t>US Strait JDF</t>
+  </si>
+  <si>
+    <t>Quillayute</t>
+  </si>
+  <si>
+    <t>omu</t>
+  </si>
+  <si>
+    <t>US Outside</t>
+  </si>
+  <si>
+    <t>Hoh</t>
+  </si>
+  <si>
+    <t>Queets</t>
+  </si>
+  <si>
+    <t>Grays Harbor</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>fixed</t>
+  </si>
+  <si>
+    <t>Canada Fixed</t>
+  </si>
+  <si>
+    <t>Georgia Strait ML</t>
+  </si>
+  <si>
+    <t>Georgia Strait VI</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>StockID</t>
+  </si>
+  <si>
+    <t>Upper Abundance Cohort</t>
+  </si>
+  <si>
+    <t>Lower Abundance Cohort</t>
+  </si>
+  <si>
+    <t>Low Abundance Management Objective</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>Moderate Abundance Management Objective</t>
+  </si>
+  <si>
+    <t>Abundant Abundance Management Objective</t>
+  </si>
+  <si>
+    <t>Lower Escapement Goal</t>
+  </si>
+  <si>
+    <t>Upper Escapement Goal</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>Cap Method</t>
   </si>
 </sst>
 </file>
@@ -981,6 +1078,1506 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FA2F8A4-2609-4EE6-A53A-ADC42F7FF467}">
+  <dimension ref="A1:L39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="14.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E1" t="s">
+        <v>180</v>
+      </c>
+      <c r="F1" t="s">
+        <v>189</v>
+      </c>
+      <c r="G1" t="s">
+        <v>182</v>
+      </c>
+      <c r="H1" t="s">
+        <v>184</v>
+      </c>
+      <c r="I1" t="s">
+        <v>185</v>
+      </c>
+      <c r="J1" t="s">
+        <v>186</v>
+      </c>
+      <c r="K1" t="s">
+        <v>187</v>
+      </c>
+      <c r="L1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D2">
+        <v>22857</v>
+      </c>
+      <c r="E2">
+        <v>62500</v>
+      </c>
+      <c r="F2" t="s">
+        <v>160</v>
+      </c>
+      <c r="G2">
+        <v>0.2</v>
+      </c>
+      <c r="H2">
+        <v>0.35</v>
+      </c>
+      <c r="I2">
+        <v>0.6</v>
+      </c>
+      <c r="J2" t="s">
+        <v>161</v>
+      </c>
+      <c r="K2" t="s">
+        <v>161</v>
+      </c>
+      <c r="L2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>159</v>
+      </c>
+      <c r="D3">
+        <v>22857</v>
+      </c>
+      <c r="E3">
+        <v>62500</v>
+      </c>
+      <c r="F3" t="s">
+        <v>160</v>
+      </c>
+      <c r="G3">
+        <v>0.2</v>
+      </c>
+      <c r="H3">
+        <v>0.35</v>
+      </c>
+      <c r="I3">
+        <v>0.6</v>
+      </c>
+      <c r="J3" t="s">
+        <v>161</v>
+      </c>
+      <c r="K3" t="s">
+        <v>161</v>
+      </c>
+      <c r="L3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>159</v>
+      </c>
+      <c r="D4">
+        <v>22857</v>
+      </c>
+      <c r="E4">
+        <v>62500</v>
+      </c>
+      <c r="F4" t="s">
+        <v>160</v>
+      </c>
+      <c r="G4">
+        <v>0.2</v>
+      </c>
+      <c r="H4">
+        <v>0.35</v>
+      </c>
+      <c r="I4">
+        <v>0.6</v>
+      </c>
+      <c r="J4" t="s">
+        <v>161</v>
+      </c>
+      <c r="K4" t="s">
+        <v>161</v>
+      </c>
+      <c r="L4" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>159</v>
+      </c>
+      <c r="D5">
+        <v>22857</v>
+      </c>
+      <c r="E5">
+        <v>62500</v>
+      </c>
+      <c r="F5" t="s">
+        <v>160</v>
+      </c>
+      <c r="G5">
+        <v>0.2</v>
+      </c>
+      <c r="H5">
+        <v>0.35</v>
+      </c>
+      <c r="I5">
+        <v>0.6</v>
+      </c>
+      <c r="J5" t="s">
+        <v>161</v>
+      </c>
+      <c r="K5" t="s">
+        <v>161</v>
+      </c>
+      <c r="L5" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
+        <v>163</v>
+      </c>
+      <c r="D6">
+        <v>9385</v>
+      </c>
+      <c r="E6">
+        <v>20000</v>
+      </c>
+      <c r="F6" t="s">
+        <v>160</v>
+      </c>
+      <c r="G6">
+        <v>0.2</v>
+      </c>
+      <c r="H6">
+        <v>0.35</v>
+      </c>
+      <c r="I6">
+        <v>0.5</v>
+      </c>
+      <c r="J6" t="s">
+        <v>161</v>
+      </c>
+      <c r="K6" t="s">
+        <v>161</v>
+      </c>
+      <c r="L6" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
+        <v>163</v>
+      </c>
+      <c r="D7">
+        <v>9385</v>
+      </c>
+      <c r="E7">
+        <v>20000</v>
+      </c>
+      <c r="F7" t="s">
+        <v>160</v>
+      </c>
+      <c r="G7">
+        <v>0.2</v>
+      </c>
+      <c r="H7">
+        <v>0.35</v>
+      </c>
+      <c r="I7">
+        <v>0.5</v>
+      </c>
+      <c r="J7" t="s">
+        <v>161</v>
+      </c>
+      <c r="K7" t="s">
+        <v>161</v>
+      </c>
+      <c r="L7" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>35</v>
+      </c>
+      <c r="C8" t="s">
+        <v>164</v>
+      </c>
+      <c r="D8">
+        <v>51667</v>
+      </c>
+      <c r="E8">
+        <v>125000</v>
+      </c>
+      <c r="F8" t="s">
+        <v>160</v>
+      </c>
+      <c r="G8">
+        <v>0.2</v>
+      </c>
+      <c r="H8">
+        <v>0.4</v>
+      </c>
+      <c r="I8">
+        <v>0.6</v>
+      </c>
+      <c r="J8" t="s">
+        <v>161</v>
+      </c>
+      <c r="K8" t="s">
+        <v>161</v>
+      </c>
+      <c r="L8" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9">
+        <v>36</v>
+      </c>
+      <c r="C9" t="s">
+        <v>164</v>
+      </c>
+      <c r="D9">
+        <v>51667</v>
+      </c>
+      <c r="E9">
+        <v>125000</v>
+      </c>
+      <c r="F9" t="s">
+        <v>160</v>
+      </c>
+      <c r="G9">
+        <v>0.2</v>
+      </c>
+      <c r="H9">
+        <v>0.4</v>
+      </c>
+      <c r="I9">
+        <v>0.6</v>
+      </c>
+      <c r="J9" t="s">
+        <v>161</v>
+      </c>
+      <c r="K9" t="s">
+        <v>161</v>
+      </c>
+      <c r="L9" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>4</v>
+      </c>
+      <c r="B10">
+        <v>45</v>
+      </c>
+      <c r="C10" t="s">
+        <v>165</v>
+      </c>
+      <c r="D10">
+        <v>19545</v>
+      </c>
+      <c r="E10">
+        <v>41000</v>
+      </c>
+      <c r="F10" t="s">
+        <v>160</v>
+      </c>
+      <c r="G10">
+        <v>0.2</v>
+      </c>
+      <c r="H10">
+        <v>0.45</v>
+      </c>
+      <c r="I10">
+        <v>0.65</v>
+      </c>
+      <c r="J10" t="s">
+        <v>161</v>
+      </c>
+      <c r="K10" t="s">
+        <v>161</v>
+      </c>
+      <c r="L10" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>4</v>
+      </c>
+      <c r="B11">
+        <v>46</v>
+      </c>
+      <c r="C11" t="s">
+        <v>165</v>
+      </c>
+      <c r="D11">
+        <v>19545</v>
+      </c>
+      <c r="E11">
+        <v>41000</v>
+      </c>
+      <c r="F11" t="s">
+        <v>160</v>
+      </c>
+      <c r="G11">
+        <v>0.2</v>
+      </c>
+      <c r="H11">
+        <v>0.45</v>
+      </c>
+      <c r="I11">
+        <v>0.65</v>
+      </c>
+      <c r="J11" t="s">
+        <v>161</v>
+      </c>
+      <c r="K11" t="s">
+        <v>161</v>
+      </c>
+      <c r="L11" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>4</v>
+      </c>
+      <c r="B12">
+        <v>55</v>
+      </c>
+      <c r="C12" t="s">
+        <v>165</v>
+      </c>
+      <c r="D12">
+        <v>19545</v>
+      </c>
+      <c r="E12">
+        <v>41000</v>
+      </c>
+      <c r="F12" t="s">
+        <v>160</v>
+      </c>
+      <c r="G12">
+        <v>0.2</v>
+      </c>
+      <c r="H12">
+        <v>0.45</v>
+      </c>
+      <c r="I12">
+        <v>0.65</v>
+      </c>
+      <c r="J12" t="s">
+        <v>161</v>
+      </c>
+      <c r="K12" t="s">
+        <v>161</v>
+      </c>
+      <c r="L12" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>4</v>
+      </c>
+      <c r="B13">
+        <v>56</v>
+      </c>
+      <c r="C13" t="s">
+        <v>165</v>
+      </c>
+      <c r="D13">
+        <v>19545</v>
+      </c>
+      <c r="E13">
+        <v>41000</v>
+      </c>
+      <c r="F13" t="s">
+        <v>160</v>
+      </c>
+      <c r="G13">
+        <v>0.2</v>
+      </c>
+      <c r="H13">
+        <v>0.45</v>
+      </c>
+      <c r="I13">
+        <v>0.65</v>
+      </c>
+      <c r="J13" t="s">
+        <v>161</v>
+      </c>
+      <c r="K13" t="s">
+        <v>161</v>
+      </c>
+      <c r="L13" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>4</v>
+      </c>
+      <c r="B14">
+        <v>59</v>
+      </c>
+      <c r="C14" t="s">
+        <v>165</v>
+      </c>
+      <c r="D14">
+        <v>19545</v>
+      </c>
+      <c r="E14">
+        <v>41000</v>
+      </c>
+      <c r="F14" t="s">
+        <v>160</v>
+      </c>
+      <c r="G14">
+        <v>0.2</v>
+      </c>
+      <c r="H14">
+        <v>0.45</v>
+      </c>
+      <c r="I14">
+        <v>0.65</v>
+      </c>
+      <c r="J14" t="s">
+        <v>161</v>
+      </c>
+      <c r="K14" t="s">
+        <v>161</v>
+      </c>
+      <c r="L14" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>4</v>
+      </c>
+      <c r="B15">
+        <v>60</v>
+      </c>
+      <c r="C15" t="s">
+        <v>165</v>
+      </c>
+      <c r="D15">
+        <v>19545</v>
+      </c>
+      <c r="E15">
+        <v>41000</v>
+      </c>
+      <c r="F15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G15">
+        <v>0.2</v>
+      </c>
+      <c r="H15">
+        <v>0.45</v>
+      </c>
+      <c r="I15">
+        <v>0.65</v>
+      </c>
+      <c r="J15" t="s">
+        <v>161</v>
+      </c>
+      <c r="K15" t="s">
+        <v>161</v>
+      </c>
+      <c r="L15" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>5</v>
+      </c>
+      <c r="B16">
+        <v>115</v>
+      </c>
+      <c r="C16" t="s">
+        <v>166</v>
+      </c>
+      <c r="D16">
+        <v>11679</v>
+      </c>
+      <c r="E16">
+        <v>27445</v>
+      </c>
+      <c r="F16" t="s">
+        <v>160</v>
+      </c>
+      <c r="G16">
+        <v>0.2</v>
+      </c>
+      <c r="H16">
+        <v>0.4</v>
+      </c>
+      <c r="I16">
+        <v>0.6</v>
+      </c>
+      <c r="J16" t="s">
+        <v>161</v>
+      </c>
+      <c r="K16" t="s">
+        <v>161</v>
+      </c>
+      <c r="L16" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>5</v>
+      </c>
+      <c r="B17">
+        <v>116</v>
+      </c>
+      <c r="C17" t="s">
+        <v>166</v>
+      </c>
+      <c r="D17">
+        <v>11679</v>
+      </c>
+      <c r="E17">
+        <v>27445</v>
+      </c>
+      <c r="F17" t="s">
+        <v>160</v>
+      </c>
+      <c r="G17">
+        <v>0.2</v>
+      </c>
+      <c r="H17">
+        <v>0.4</v>
+      </c>
+      <c r="I17">
+        <v>0.6</v>
+      </c>
+      <c r="J17" t="s">
+        <v>161</v>
+      </c>
+      <c r="K17" t="s">
+        <v>161</v>
+      </c>
+      <c r="L17" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>5</v>
+      </c>
+      <c r="B18">
+        <v>117</v>
+      </c>
+      <c r="C18" t="s">
+        <v>166</v>
+      </c>
+      <c r="D18">
+        <v>11679</v>
+      </c>
+      <c r="E18">
+        <v>27445</v>
+      </c>
+      <c r="F18" t="s">
+        <v>160</v>
+      </c>
+      <c r="G18">
+        <v>0.2</v>
+      </c>
+      <c r="H18">
+        <v>0.4</v>
+      </c>
+      <c r="I18">
+        <v>0.6</v>
+      </c>
+      <c r="J18" t="s">
+        <v>161</v>
+      </c>
+      <c r="K18" t="s">
+        <v>161</v>
+      </c>
+      <c r="L18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>5</v>
+      </c>
+      <c r="B19">
+        <v>118</v>
+      </c>
+      <c r="C19" t="s">
+        <v>166</v>
+      </c>
+      <c r="D19">
+        <v>11679</v>
+      </c>
+      <c r="E19">
+        <v>27445</v>
+      </c>
+      <c r="F19" t="s">
+        <v>160</v>
+      </c>
+      <c r="G19">
+        <v>0.2</v>
+      </c>
+      <c r="H19">
+        <v>0.4</v>
+      </c>
+      <c r="I19">
+        <v>0.6</v>
+      </c>
+      <c r="J19" t="s">
+        <v>161</v>
+      </c>
+      <c r="K19" t="s">
+        <v>161</v>
+      </c>
+      <c r="L19" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>6</v>
+      </c>
+      <c r="B20">
+        <v>131</v>
+      </c>
+      <c r="C20" t="s">
+        <v>167</v>
+      </c>
+      <c r="D20">
+        <v>7875</v>
+      </c>
+      <c r="E20">
+        <v>10500</v>
+      </c>
+      <c r="F20" t="s">
+        <v>168</v>
+      </c>
+      <c r="G20">
+        <v>0.2</v>
+      </c>
+      <c r="H20" t="s">
+        <v>161</v>
+      </c>
+      <c r="I20" t="s">
+        <v>161</v>
+      </c>
+      <c r="J20">
+        <v>6300</v>
+      </c>
+      <c r="K20">
+        <v>15800</v>
+      </c>
+      <c r="L20" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>6</v>
+      </c>
+      <c r="B21">
+        <v>132</v>
+      </c>
+      <c r="C21" t="s">
+        <v>167</v>
+      </c>
+      <c r="D21">
+        <v>7875</v>
+      </c>
+      <c r="E21">
+        <v>10500</v>
+      </c>
+      <c r="F21" t="s">
+        <v>168</v>
+      </c>
+      <c r="G21">
+        <v>0.2</v>
+      </c>
+      <c r="H21" t="s">
+        <v>161</v>
+      </c>
+      <c r="I21" t="s">
+        <v>161</v>
+      </c>
+      <c r="J21">
+        <v>6300</v>
+      </c>
+      <c r="K21">
+        <v>15800</v>
+      </c>
+      <c r="L21" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>7</v>
+      </c>
+      <c r="B22">
+        <v>135</v>
+      </c>
+      <c r="C22" t="s">
+        <v>170</v>
+      </c>
+      <c r="D22">
+        <v>2500</v>
+      </c>
+      <c r="E22">
+        <v>3333</v>
+      </c>
+      <c r="F22" t="s">
+        <v>168</v>
+      </c>
+      <c r="G22">
+        <v>0.2</v>
+      </c>
+      <c r="H22" t="s">
+        <v>161</v>
+      </c>
+      <c r="I22" t="s">
+        <v>161</v>
+      </c>
+      <c r="J22">
+        <v>2000</v>
+      </c>
+      <c r="K22">
+        <v>5000</v>
+      </c>
+      <c r="L22" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>7</v>
+      </c>
+      <c r="B23">
+        <v>136</v>
+      </c>
+      <c r="C23" t="s">
+        <v>170</v>
+      </c>
+      <c r="D23">
+        <v>2500</v>
+      </c>
+      <c r="E23">
+        <v>3333</v>
+      </c>
+      <c r="F23" t="s">
+        <v>168</v>
+      </c>
+      <c r="G23">
+        <v>0.2</v>
+      </c>
+      <c r="H23" t="s">
+        <v>161</v>
+      </c>
+      <c r="I23" t="s">
+        <v>161</v>
+      </c>
+      <c r="J23">
+        <v>2000</v>
+      </c>
+      <c r="K23">
+        <v>5000</v>
+      </c>
+      <c r="L23" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>8</v>
+      </c>
+      <c r="B24">
+        <v>139</v>
+      </c>
+      <c r="C24" t="s">
+        <v>171</v>
+      </c>
+      <c r="D24">
+        <v>7250</v>
+      </c>
+      <c r="E24">
+        <v>9667</v>
+      </c>
+      <c r="F24" t="s">
+        <v>168</v>
+      </c>
+      <c r="G24">
+        <v>0.2</v>
+      </c>
+      <c r="H24" t="s">
+        <v>161</v>
+      </c>
+      <c r="I24" t="s">
+        <v>161</v>
+      </c>
+      <c r="J24">
+        <v>5800</v>
+      </c>
+      <c r="K24">
+        <v>14500</v>
+      </c>
+      <c r="L24" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>8</v>
+      </c>
+      <c r="B25">
+        <v>140</v>
+      </c>
+      <c r="C25" t="s">
+        <v>171</v>
+      </c>
+      <c r="D25">
+        <v>7250</v>
+      </c>
+      <c r="E25">
+        <v>9667</v>
+      </c>
+      <c r="F25" t="s">
+        <v>168</v>
+      </c>
+      <c r="G25">
+        <v>0.2</v>
+      </c>
+      <c r="H25" t="s">
+        <v>161</v>
+      </c>
+      <c r="I25" t="s">
+        <v>161</v>
+      </c>
+      <c r="J25">
+        <v>5800</v>
+      </c>
+      <c r="K25">
+        <v>14500</v>
+      </c>
+      <c r="L25" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>9</v>
+      </c>
+      <c r="B26">
+        <v>149</v>
+      </c>
+      <c r="C26" t="s">
+        <v>172</v>
+      </c>
+      <c r="D26">
+        <v>44250</v>
+      </c>
+      <c r="E26">
+        <v>59000</v>
+      </c>
+      <c r="F26" t="s">
+        <v>168</v>
+      </c>
+      <c r="G26" t="s">
+        <v>161</v>
+      </c>
+      <c r="H26" t="s">
+        <v>161</v>
+      </c>
+      <c r="I26">
+        <v>0.6</v>
+      </c>
+      <c r="J26">
+        <v>35400</v>
+      </c>
+      <c r="K26">
+        <v>35400</v>
+      </c>
+      <c r="L26" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>9</v>
+      </c>
+      <c r="B27">
+        <v>150</v>
+      </c>
+      <c r="C27" t="s">
+        <v>172</v>
+      </c>
+      <c r="D27">
+        <v>44250</v>
+      </c>
+      <c r="E27">
+        <v>59000</v>
+      </c>
+      <c r="F27" t="s">
+        <v>168</v>
+      </c>
+      <c r="G27" t="s">
+        <v>161</v>
+      </c>
+      <c r="H27" t="s">
+        <v>161</v>
+      </c>
+      <c r="I27">
+        <v>0.6</v>
+      </c>
+      <c r="J27">
+        <v>35400</v>
+      </c>
+      <c r="K27">
+        <v>35400</v>
+      </c>
+      <c r="L27" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>9</v>
+      </c>
+      <c r="B28">
+        <v>153</v>
+      </c>
+      <c r="C28" t="s">
+        <v>172</v>
+      </c>
+      <c r="D28">
+        <v>44250</v>
+      </c>
+      <c r="E28">
+        <v>59000</v>
+      </c>
+      <c r="F28" t="s">
+        <v>168</v>
+      </c>
+      <c r="G28" t="s">
+        <v>161</v>
+      </c>
+      <c r="H28" t="s">
+        <v>161</v>
+      </c>
+      <c r="I28">
+        <v>0.6</v>
+      </c>
+      <c r="J28">
+        <v>35400</v>
+      </c>
+      <c r="K28">
+        <v>35400</v>
+      </c>
+      <c r="L28" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>9</v>
+      </c>
+      <c r="B29">
+        <v>154</v>
+      </c>
+      <c r="C29" t="s">
+        <v>172</v>
+      </c>
+      <c r="D29">
+        <v>44250</v>
+      </c>
+      <c r="E29">
+        <v>59000</v>
+      </c>
+      <c r="F29" t="s">
+        <v>168</v>
+      </c>
+      <c r="G29" t="s">
+        <v>161</v>
+      </c>
+      <c r="H29" t="s">
+        <v>161</v>
+      </c>
+      <c r="I29">
+        <v>0.6</v>
+      </c>
+      <c r="J29">
+        <v>35400</v>
+      </c>
+      <c r="K29">
+        <v>35400</v>
+      </c>
+      <c r="L29" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>9</v>
+      </c>
+      <c r="B30">
+        <v>157</v>
+      </c>
+      <c r="C30" t="s">
+        <v>172</v>
+      </c>
+      <c r="D30">
+        <v>44250</v>
+      </c>
+      <c r="E30">
+        <v>59000</v>
+      </c>
+      <c r="F30" t="s">
+        <v>168</v>
+      </c>
+      <c r="G30" t="s">
+        <v>161</v>
+      </c>
+      <c r="H30" t="s">
+        <v>161</v>
+      </c>
+      <c r="I30">
+        <v>0.6</v>
+      </c>
+      <c r="J30">
+        <v>35400</v>
+      </c>
+      <c r="K30">
+        <v>35400</v>
+      </c>
+      <c r="L30" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>9</v>
+      </c>
+      <c r="B31">
+        <v>158</v>
+      </c>
+      <c r="C31" t="s">
+        <v>172</v>
+      </c>
+      <c r="D31">
+        <v>44250</v>
+      </c>
+      <c r="E31">
+        <v>59000</v>
+      </c>
+      <c r="F31" t="s">
+        <v>168</v>
+      </c>
+      <c r="G31" t="s">
+        <v>161</v>
+      </c>
+      <c r="H31" t="s">
+        <v>161</v>
+      </c>
+      <c r="I31">
+        <v>0.6</v>
+      </c>
+      <c r="J31">
+        <v>35400</v>
+      </c>
+      <c r="K31">
+        <v>35400</v>
+      </c>
+      <c r="L31" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>10</v>
+      </c>
+      <c r="B32">
+        <v>227</v>
+      </c>
+      <c r="C32" t="s">
+        <v>40</v>
+      </c>
+      <c r="D32" t="s">
+        <v>161</v>
+      </c>
+      <c r="E32" t="s">
+        <v>161</v>
+      </c>
+      <c r="F32" t="s">
+        <v>183</v>
+      </c>
+      <c r="G32" t="s">
+        <v>161</v>
+      </c>
+      <c r="H32" t="s">
+        <v>161</v>
+      </c>
+      <c r="I32" t="s">
+        <v>161</v>
+      </c>
+      <c r="J32" t="s">
+        <v>161</v>
+      </c>
+      <c r="K32" t="s">
+        <v>161</v>
+      </c>
+      <c r="L32" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>10</v>
+      </c>
+      <c r="B33">
+        <v>228</v>
+      </c>
+      <c r="C33" t="s">
+        <v>40</v>
+      </c>
+      <c r="D33" t="s">
+        <v>161</v>
+      </c>
+      <c r="E33" t="s">
+        <v>161</v>
+      </c>
+      <c r="F33" t="s">
+        <v>183</v>
+      </c>
+      <c r="G33" t="s">
+        <v>161</v>
+      </c>
+      <c r="H33" t="s">
+        <v>161</v>
+      </c>
+      <c r="I33" t="s">
+        <v>161</v>
+      </c>
+      <c r="J33" t="s">
+        <v>161</v>
+      </c>
+      <c r="K33" t="s">
+        <v>161</v>
+      </c>
+      <c r="L33" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>11</v>
+      </c>
+      <c r="B34">
+        <v>231</v>
+      </c>
+      <c r="C34" t="s">
+        <v>44</v>
+      </c>
+      <c r="D34" t="s">
+        <v>161</v>
+      </c>
+      <c r="E34" t="s">
+        <v>161</v>
+      </c>
+      <c r="F34" t="s">
+        <v>174</v>
+      </c>
+      <c r="G34">
+        <v>0.2</v>
+      </c>
+      <c r="H34" t="s">
+        <v>161</v>
+      </c>
+      <c r="I34" t="s">
+        <v>161</v>
+      </c>
+      <c r="J34" t="s">
+        <v>161</v>
+      </c>
+      <c r="K34" t="s">
+        <v>161</v>
+      </c>
+      <c r="L34" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>11</v>
+      </c>
+      <c r="B35">
+        <v>232</v>
+      </c>
+      <c r="C35" t="s">
+        <v>44</v>
+      </c>
+      <c r="D35" t="s">
+        <v>161</v>
+      </c>
+      <c r="E35" t="s">
+        <v>161</v>
+      </c>
+      <c r="F35" t="s">
+        <v>174</v>
+      </c>
+      <c r="G35">
+        <v>0.2</v>
+      </c>
+      <c r="H35" t="s">
+        <v>161</v>
+      </c>
+      <c r="I35" t="s">
+        <v>161</v>
+      </c>
+      <c r="J35" t="s">
+        <v>161</v>
+      </c>
+      <c r="K35" t="s">
+        <v>161</v>
+      </c>
+      <c r="L35" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>12</v>
+      </c>
+      <c r="B36">
+        <v>207</v>
+      </c>
+      <c r="C36" t="s">
+        <v>176</v>
+      </c>
+      <c r="D36" t="s">
+        <v>161</v>
+      </c>
+      <c r="E36" t="s">
+        <v>161</v>
+      </c>
+      <c r="F36" t="s">
+        <v>183</v>
+      </c>
+      <c r="G36" t="s">
+        <v>161</v>
+      </c>
+      <c r="H36" t="s">
+        <v>161</v>
+      </c>
+      <c r="I36" t="s">
+        <v>161</v>
+      </c>
+      <c r="J36" t="s">
+        <v>161</v>
+      </c>
+      <c r="K36" t="s">
+        <v>161</v>
+      </c>
+      <c r="L36" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>12</v>
+      </c>
+      <c r="B37">
+        <v>208</v>
+      </c>
+      <c r="C37" t="s">
+        <v>176</v>
+      </c>
+      <c r="D37" t="s">
+        <v>161</v>
+      </c>
+      <c r="E37" t="s">
+        <v>161</v>
+      </c>
+      <c r="F37" t="s">
+        <v>183</v>
+      </c>
+      <c r="G37" t="s">
+        <v>161</v>
+      </c>
+      <c r="H37" t="s">
+        <v>161</v>
+      </c>
+      <c r="I37" t="s">
+        <v>161</v>
+      </c>
+      <c r="J37" t="s">
+        <v>161</v>
+      </c>
+      <c r="K37" t="s">
+        <v>161</v>
+      </c>
+      <c r="L37" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>13</v>
+      </c>
+      <c r="B38">
+        <v>211</v>
+      </c>
+      <c r="C38" t="s">
+        <v>177</v>
+      </c>
+      <c r="D38" t="s">
+        <v>161</v>
+      </c>
+      <c r="E38" t="s">
+        <v>161</v>
+      </c>
+      <c r="F38" t="s">
+        <v>183</v>
+      </c>
+      <c r="G38" t="s">
+        <v>161</v>
+      </c>
+      <c r="H38" t="s">
+        <v>161</v>
+      </c>
+      <c r="I38" t="s">
+        <v>161</v>
+      </c>
+      <c r="J38" t="s">
+        <v>161</v>
+      </c>
+      <c r="K38" t="s">
+        <v>161</v>
+      </c>
+      <c r="L38" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>13</v>
+      </c>
+      <c r="B39">
+        <v>212</v>
+      </c>
+      <c r="C39" t="s">
+        <v>177</v>
+      </c>
+      <c r="D39" t="s">
+        <v>161</v>
+      </c>
+      <c r="E39" t="s">
+        <v>161</v>
+      </c>
+      <c r="F39" t="s">
+        <v>183</v>
+      </c>
+      <c r="G39" t="s">
+        <v>161</v>
+      </c>
+      <c r="H39" t="s">
+        <v>161</v>
+      </c>
+      <c r="I39" t="s">
+        <v>161</v>
+      </c>
+      <c r="J39" t="s">
+        <v>161</v>
+      </c>
+      <c r="K39" t="s">
+        <v>161</v>
+      </c>
+      <c r="L39" t="s">
+        <v>173</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F8"/>
   <sheetViews>
@@ -1158,7 +2755,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B13"/>
   <sheetViews>
@@ -1266,11 +2863,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
move members, add acronyms with links, clean up setup and demo some figs and tables
</commit_message>
<xml_diff>
--- a/StaticTables.xlsx
+++ b/StaticTables.xlsx
@@ -8,28 +8,37 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stateofwa-my.sharepoint.com/personal/daniel_auerbach_dfw_wa_gov/Documents/code/PeriodicReport/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="44" documentId="13_ncr:1_{793868AE-9DA0-439D-B941-FC5A2F22A4BB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{E2757023-91D6-413D-8147-473D2925A4D1}"/>
+  <xr:revisionPtr revIDLastSave="121" documentId="13_ncr:1_{793868AE-9DA0-439D-B941-FC5A2F22A4BB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{8DB362CD-B9FC-4018-A61F-EA166A48FCF3}"/>
   <bookViews>
-    <workbookView xWindow="924" yWindow="324" windowWidth="19872" windowHeight="11712" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-15410" yWindow="-19670" windowWidth="33330" windowHeight="16960" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="members" sheetId="5" r:id="rId1"/>
     <sheet name="lu_stock" sheetId="6" r:id="rId2"/>
     <sheet name="RunFiles" sheetId="1" r:id="rId3"/>
     <sheet name="CUs" sheetId="2" r:id="rId4"/>
-    <sheet name="Acronyms" sheetId="3" r:id="rId5"/>
+    <sheet name="acronyms" sheetId="3" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="205">
   <si>
     <t>BK04.Cmd</t>
   </si>
@@ -136,21 +145,9 @@
     <t>WSP Conservation Unit Component</t>
   </si>
   <si>
-    <t xml:space="preserve">  </t>
-  </si>
-  <si>
-    <t>:-------</t>
-  </si>
-  <si>
-    <t>:-------------</t>
-  </si>
-  <si>
     <t>Boundary Bay</t>
   </si>
   <si>
-    <t xml:space="preserve">   </t>
-  </si>
-  <si>
     <t>Lower Fraser</t>
   </si>
   <si>
@@ -193,261 +190,6 @@
     <t>East Vancouver Island – Georgia Strait</t>
   </si>
   <si>
-    <t xml:space="preserve"> ABM </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Abundance-Based Management </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> B.C.  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> British Columbia    </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> BY     </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Brood Year      </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> [CDFO](https://www.dfo-mpo.gc.ca/index-eng.htm) </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Canadian Department of Fisheries and Oceans</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> [CoTC](https://www.psc.org/about-us/structure/committees/technical/coho/)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Coho Joint Technical Committee      </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> CU </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Conservation Unit </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> CWT    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Coded-Wire Tag  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> DIT    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Double-Index Tag </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> EDT    </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Electronic Tag Detection </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ER     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Exploitation Rate  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> [ESA](https://www.fws.gov/international/laws-treaties-agreements/us-conservation-laws/endangered-species-act.html)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> U.S. Endangered Species Act </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> [ESU](https://www.nwfsc.noaa.gov/assets/4/6878_09172014_172219_Waples.1995.pdf)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Evolutionarily Significant Unit </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> FRAM   </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Fishery Regulation and Assessment Model </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> HC     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Hood Canal  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> MSF    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Mark-Selective Fishery  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> MSH</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Maximum Sustainable Harvest </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> MSM    </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Mixed-Stock Model  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> MU     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Management Unit  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> [NMFS](https://www.fisheries.noaa.gov/) </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> National Marine Fisheries Service </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> NSF    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Non-Selective Fishery  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> [NTC](https://nuuchahnulth.org/) </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Nuu-chah-nulth Tribal Council </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> [NWIFC](https://nwifc.org/) </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Northwest Indian Fisheries Commission </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> [ODFW](https://www.dfw.state.or.us/) </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Oregon Department of Fish and Wildlife </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> OR     </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Oregon </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> PEF </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Production Expansion Factor </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> [PFMC](https://www.pcouncil.org/)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Pacific Fisheries Management Council (U.S.) </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> PS     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Puget Sound  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> [PSC](https://www.psc.org/)    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Pacific Salmon Commission </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> [PST](https://www.psc.org/publications/pacific-salmon-treaty/)    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Pacific Salmon Treaty  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> [QIN](http://www.quinaultindiannation.com/) </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Quinault Indian Nation </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> [RMIS](https://www.rmpc.org/)   </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Regional Mark Information System  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> [RMPC](https://www.rmpc.org/)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Regional Mark Processing Center </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RRTERM </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Terminal Area Run Reconstruction Program </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> SIT</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Single Index Tag </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> SJDF   </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Strait of Juan de Fuca  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> [SUQ](https://suquamish.nsn.us/) </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Suquamish Tribe </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> [TUL](https://www.tulaliptribes-nsn.gov/) </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Tulalip Tribes </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> [UFFCA](https://www.upperfraser.ca/) </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Upper Fraser Fisheries Conservation Alliance </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> U.S. </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> United States </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> [USFWS](https://www.fws.gov/) </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> U.S. Fish and Wildlife Service </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> WA     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Washington  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> [WDFW](https://wdfw.wa.gov/) </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Washington Department of Fish and Wildlife </t>
-  </si>
-  <si>
     <t>Dr. Laurie Weitkamp, NMFS</t>
   </si>
   <si>
@@ -599,6 +341,318 @@
   </si>
   <si>
     <t>Cap Method</t>
+  </si>
+  <si>
+    <t>Acronym</t>
+  </si>
+  <si>
+    <t>Definition</t>
+  </si>
+  <si>
+    <t>Coded-Wire Tag</t>
+  </si>
+  <si>
+    <t>Exploitation Rate</t>
+  </si>
+  <si>
+    <t>Mark-Selective Fishery</t>
+  </si>
+  <si>
+    <t>Non-Selective Fishery</t>
+  </si>
+  <si>
+    <t>Pacific Salmon Treaty</t>
+  </si>
+  <si>
+    <t>Washington</t>
+  </si>
+  <si>
+    <t>ABM</t>
+  </si>
+  <si>
+    <t>B.C.</t>
+  </si>
+  <si>
+    <t>BY</t>
+  </si>
+  <si>
+    <t>CU</t>
+  </si>
+  <si>
+    <t>CWT</t>
+  </si>
+  <si>
+    <t>DIT</t>
+  </si>
+  <si>
+    <t>EDT</t>
+  </si>
+  <si>
+    <t>ER</t>
+  </si>
+  <si>
+    <t>FRAM</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>MSF</t>
+  </si>
+  <si>
+    <t>MSH</t>
+  </si>
+  <si>
+    <t>MSM</t>
+  </si>
+  <si>
+    <t>MU</t>
+  </si>
+  <si>
+    <t>NSF</t>
+  </si>
+  <si>
+    <t>OR</t>
+  </si>
+  <si>
+    <t>PEF</t>
+  </si>
+  <si>
+    <t>PS</t>
+  </si>
+  <si>
+    <t>RRTERM</t>
+  </si>
+  <si>
+    <t>SIT</t>
+  </si>
+  <si>
+    <t>SJDF</t>
+  </si>
+  <si>
+    <t>U.S.</t>
+  </si>
+  <si>
+    <t>WA</t>
+  </si>
+  <si>
+    <t>Abundance-Based Management</t>
+  </si>
+  <si>
+    <t>British Columbia</t>
+  </si>
+  <si>
+    <t>Brood Year</t>
+  </si>
+  <si>
+    <t>Canadian Department of Fisheries and Oceans</t>
+  </si>
+  <si>
+    <t>Coho Joint Technical Committee</t>
+  </si>
+  <si>
+    <t>Conservation Unit</t>
+  </si>
+  <si>
+    <t>Double-Index Tag</t>
+  </si>
+  <si>
+    <t>Electronic Tag Detection</t>
+  </si>
+  <si>
+    <t>U.S. Endangered Species Act</t>
+  </si>
+  <si>
+    <t>Evolutionarily Significant Unit</t>
+  </si>
+  <si>
+    <t>Fishery Regulation and Assessment Model</t>
+  </si>
+  <si>
+    <t>Maximum Sustainable Harvest</t>
+  </si>
+  <si>
+    <t>Mixed-Stock Model</t>
+  </si>
+  <si>
+    <t>National Marine Fisheries Service</t>
+  </si>
+  <si>
+    <t>Nuu-chah-nulth Tribal Council</t>
+  </si>
+  <si>
+    <t>Northwest Indian Fisheries Commission</t>
+  </si>
+  <si>
+    <t>Oregon Department of Fish and Wildlife</t>
+  </si>
+  <si>
+    <t>Oregon</t>
+  </si>
+  <si>
+    <t>Production Expansion Factor</t>
+  </si>
+  <si>
+    <t>Puget Sound</t>
+  </si>
+  <si>
+    <t>Pacific Salmon Commission</t>
+  </si>
+  <si>
+    <t>Quinault Indian Nation</t>
+  </si>
+  <si>
+    <t>Regional Mark Information System</t>
+  </si>
+  <si>
+    <t>Regional Mark Processing Center</t>
+  </si>
+  <si>
+    <t>Terminal Area Run Reconstruction Program</t>
+  </si>
+  <si>
+    <t>Single Index Tag</t>
+  </si>
+  <si>
+    <t>Strait of Juan de Fuca</t>
+  </si>
+  <si>
+    <t>Suquamish Tribe</t>
+  </si>
+  <si>
+    <t>Tulalip Tribes</t>
+  </si>
+  <si>
+    <t>Upper Fraser Fisheries Conservation Alliance</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>U.S. Fish and Wildlife Service</t>
+  </si>
+  <si>
+    <t>Washington Department of Fish and Wildlife</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>https://www.dfo-mpo.gc.ca/index-eng.htm</t>
+  </si>
+  <si>
+    <t>https://www.psc.org/about-us/structure/committees/technical/coho/</t>
+  </si>
+  <si>
+    <t>https://www.fws.gov/international/laws-treaties-agreements/us-conservation-laws/endangered-species-act.html</t>
+  </si>
+  <si>
+    <t>https://www.nwfsc.noaa.gov/assets/4/6878_09172014_172219_Waples.1995.pdf</t>
+  </si>
+  <si>
+    <t>https://www.fisheries.noaa.gov/</t>
+  </si>
+  <si>
+    <t>https://nuuchahnulth.org/</t>
+  </si>
+  <si>
+    <t>https://nwifc.org/</t>
+  </si>
+  <si>
+    <t>https://www.dfw.state.or.us/</t>
+  </si>
+  <si>
+    <t>Pacific Fisheries Management Council U.S.</t>
+  </si>
+  <si>
+    <t>https://www.pcouncil.org/</t>
+  </si>
+  <si>
+    <t>https://www.psc.org/</t>
+  </si>
+  <si>
+    <t>https://www.psc.org/publications/pacific-salmon-treaty/</t>
+  </si>
+  <si>
+    <t>http://www.quinaultindiannation.com/</t>
+  </si>
+  <si>
+    <t>https://www.rmpc.org/</t>
+  </si>
+  <si>
+    <t>https://suquamish.nsn.us/</t>
+  </si>
+  <si>
+    <t>https://www.tulaliptribes-nsn.gov/</t>
+  </si>
+  <si>
+    <t>https://www.upperfraser.ca/</t>
+  </si>
+  <si>
+    <t>https://www.fws.gov/</t>
+  </si>
+  <si>
+    <t>https://wdfw.wa.gov/</t>
+  </si>
+  <si>
+    <t>CDFO</t>
+  </si>
+  <si>
+    <t>CoTC</t>
+  </si>
+  <si>
+    <t>ESA</t>
+  </si>
+  <si>
+    <t>ESU</t>
+  </si>
+  <si>
+    <t>NMFS</t>
+  </si>
+  <si>
+    <t>NTC</t>
+  </si>
+  <si>
+    <t>NWIFC</t>
+  </si>
+  <si>
+    <t>ODFW</t>
+  </si>
+  <si>
+    <t>PFMC</t>
+  </si>
+  <si>
+    <t>PSC</t>
+  </si>
+  <si>
+    <t>PST</t>
+  </si>
+  <si>
+    <t>QIN</t>
+  </si>
+  <si>
+    <t>RMIS</t>
+  </si>
+  <si>
+    <t>RMPC</t>
+  </si>
+  <si>
+    <t>SUQ</t>
+  </si>
+  <si>
+    <t>TUL</t>
+  </si>
+  <si>
+    <t>UFFCA</t>
+  </si>
+  <si>
+    <t>USFWS</t>
+  </si>
+  <si>
+    <t>WDFW</t>
+  </si>
+  <si>
+    <t>https://framverse.github.io/fram_doc/</t>
   </si>
 </sst>
 </file>
@@ -678,7 +732,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -708,6 +762,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1002,73 +1059,73 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>152</v>
+        <v>63</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>151</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>150</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
-        <v>149</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>148</v>
+        <v>59</v>
       </c>
       <c r="B3" t="s">
-        <v>153</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>146</v>
+        <v>57</v>
       </c>
       <c r="B4" t="s">
-        <v>147</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>143</v>
+        <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>145</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>141</v>
+        <v>52</v>
       </c>
       <c r="B6" t="s">
-        <v>144</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>155</v>
+        <v>66</v>
       </c>
       <c r="B7" t="s">
-        <v>142</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>140</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>154</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>139</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1081,7 +1138,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FA2F8A4-2609-4EE6-A53A-ADC42F7FF467}">
   <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
@@ -1092,40 +1149,40 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>158</v>
+        <v>69</v>
       </c>
       <c r="B1" t="s">
-        <v>179</v>
+        <v>90</v>
       </c>
       <c r="C1" t="s">
-        <v>178</v>
+        <v>89</v>
       </c>
       <c r="D1" t="s">
-        <v>181</v>
+        <v>92</v>
       </c>
       <c r="E1" t="s">
-        <v>180</v>
+        <v>91</v>
       </c>
       <c r="F1" t="s">
-        <v>189</v>
+        <v>100</v>
       </c>
       <c r="G1" t="s">
-        <v>182</v>
+        <v>93</v>
       </c>
       <c r="H1" t="s">
-        <v>184</v>
+        <v>95</v>
       </c>
       <c r="I1" t="s">
-        <v>185</v>
+        <v>96</v>
       </c>
       <c r="J1" t="s">
-        <v>186</v>
+        <v>97</v>
       </c>
       <c r="K1" t="s">
-        <v>187</v>
+        <v>98</v>
       </c>
       <c r="L1" t="s">
-        <v>188</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
@@ -1136,7 +1193,7 @@
         <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>159</v>
+        <v>70</v>
       </c>
       <c r="D2">
         <v>22857</v>
@@ -1145,7 +1202,7 @@
         <v>62500</v>
       </c>
       <c r="F2" t="s">
-        <v>160</v>
+        <v>71</v>
       </c>
       <c r="G2">
         <v>0.2</v>
@@ -1157,13 +1214,13 @@
         <v>0.6</v>
       </c>
       <c r="J2" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="K2" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="L2" t="s">
-        <v>162</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -1174,7 +1231,7 @@
         <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>159</v>
+        <v>70</v>
       </c>
       <c r="D3">
         <v>22857</v>
@@ -1183,7 +1240,7 @@
         <v>62500</v>
       </c>
       <c r="F3" t="s">
-        <v>160</v>
+        <v>71</v>
       </c>
       <c r="G3">
         <v>0.2</v>
@@ -1195,13 +1252,13 @@
         <v>0.6</v>
       </c>
       <c r="J3" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="K3" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="L3" t="s">
-        <v>162</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -1212,7 +1269,7 @@
         <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>159</v>
+        <v>70</v>
       </c>
       <c r="D4">
         <v>22857</v>
@@ -1221,7 +1278,7 @@
         <v>62500</v>
       </c>
       <c r="F4" t="s">
-        <v>160</v>
+        <v>71</v>
       </c>
       <c r="G4">
         <v>0.2</v>
@@ -1233,13 +1290,13 @@
         <v>0.6</v>
       </c>
       <c r="J4" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="K4" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="L4" t="s">
-        <v>162</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -1250,7 +1307,7 @@
         <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>159</v>
+        <v>70</v>
       </c>
       <c r="D5">
         <v>22857</v>
@@ -1259,7 +1316,7 @@
         <v>62500</v>
       </c>
       <c r="F5" t="s">
-        <v>160</v>
+        <v>71</v>
       </c>
       <c r="G5">
         <v>0.2</v>
@@ -1271,13 +1328,13 @@
         <v>0.6</v>
       </c>
       <c r="J5" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="K5" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="L5" t="s">
-        <v>162</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
@@ -1288,7 +1345,7 @@
         <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>163</v>
+        <v>74</v>
       </c>
       <c r="D6">
         <v>9385</v>
@@ -1297,7 +1354,7 @@
         <v>20000</v>
       </c>
       <c r="F6" t="s">
-        <v>160</v>
+        <v>71</v>
       </c>
       <c r="G6">
         <v>0.2</v>
@@ -1309,13 +1366,13 @@
         <v>0.5</v>
       </c>
       <c r="J6" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="K6" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="L6" t="s">
-        <v>162</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
@@ -1326,7 +1383,7 @@
         <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>163</v>
+        <v>74</v>
       </c>
       <c r="D7">
         <v>9385</v>
@@ -1335,7 +1392,7 @@
         <v>20000</v>
       </c>
       <c r="F7" t="s">
-        <v>160</v>
+        <v>71</v>
       </c>
       <c r="G7">
         <v>0.2</v>
@@ -1347,13 +1404,13 @@
         <v>0.5</v>
       </c>
       <c r="J7" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="K7" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="L7" t="s">
-        <v>162</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
@@ -1364,7 +1421,7 @@
         <v>35</v>
       </c>
       <c r="C8" t="s">
-        <v>164</v>
+        <v>75</v>
       </c>
       <c r="D8">
         <v>51667</v>
@@ -1373,7 +1430,7 @@
         <v>125000</v>
       </c>
       <c r="F8" t="s">
-        <v>160</v>
+        <v>71</v>
       </c>
       <c r="G8">
         <v>0.2</v>
@@ -1385,13 +1442,13 @@
         <v>0.6</v>
       </c>
       <c r="J8" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="K8" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="L8" t="s">
-        <v>162</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
@@ -1402,7 +1459,7 @@
         <v>36</v>
       </c>
       <c r="C9" t="s">
-        <v>164</v>
+        <v>75</v>
       </c>
       <c r="D9">
         <v>51667</v>
@@ -1411,7 +1468,7 @@
         <v>125000</v>
       </c>
       <c r="F9" t="s">
-        <v>160</v>
+        <v>71</v>
       </c>
       <c r="G9">
         <v>0.2</v>
@@ -1423,13 +1480,13 @@
         <v>0.6</v>
       </c>
       <c r="J9" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="K9" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="L9" t="s">
-        <v>162</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
@@ -1440,7 +1497,7 @@
         <v>45</v>
       </c>
       <c r="C10" t="s">
-        <v>165</v>
+        <v>76</v>
       </c>
       <c r="D10">
         <v>19545</v>
@@ -1449,7 +1506,7 @@
         <v>41000</v>
       </c>
       <c r="F10" t="s">
-        <v>160</v>
+        <v>71</v>
       </c>
       <c r="G10">
         <v>0.2</v>
@@ -1461,13 +1518,13 @@
         <v>0.65</v>
       </c>
       <c r="J10" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="K10" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="L10" t="s">
-        <v>162</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
@@ -1478,7 +1535,7 @@
         <v>46</v>
       </c>
       <c r="C11" t="s">
-        <v>165</v>
+        <v>76</v>
       </c>
       <c r="D11">
         <v>19545</v>
@@ -1487,7 +1544,7 @@
         <v>41000</v>
       </c>
       <c r="F11" t="s">
-        <v>160</v>
+        <v>71</v>
       </c>
       <c r="G11">
         <v>0.2</v>
@@ -1499,13 +1556,13 @@
         <v>0.65</v>
       </c>
       <c r="J11" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="K11" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="L11" t="s">
-        <v>162</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
@@ -1516,7 +1573,7 @@
         <v>55</v>
       </c>
       <c r="C12" t="s">
-        <v>165</v>
+        <v>76</v>
       </c>
       <c r="D12">
         <v>19545</v>
@@ -1525,7 +1582,7 @@
         <v>41000</v>
       </c>
       <c r="F12" t="s">
-        <v>160</v>
+        <v>71</v>
       </c>
       <c r="G12">
         <v>0.2</v>
@@ -1537,13 +1594,13 @@
         <v>0.65</v>
       </c>
       <c r="J12" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="K12" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="L12" t="s">
-        <v>162</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
@@ -1554,7 +1611,7 @@
         <v>56</v>
       </c>
       <c r="C13" t="s">
-        <v>165</v>
+        <v>76</v>
       </c>
       <c r="D13">
         <v>19545</v>
@@ -1563,7 +1620,7 @@
         <v>41000</v>
       </c>
       <c r="F13" t="s">
-        <v>160</v>
+        <v>71</v>
       </c>
       <c r="G13">
         <v>0.2</v>
@@ -1575,13 +1632,13 @@
         <v>0.65</v>
       </c>
       <c r="J13" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="K13" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="L13" t="s">
-        <v>162</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
@@ -1592,7 +1649,7 @@
         <v>59</v>
       </c>
       <c r="C14" t="s">
-        <v>165</v>
+        <v>76</v>
       </c>
       <c r="D14">
         <v>19545</v>
@@ -1601,7 +1658,7 @@
         <v>41000</v>
       </c>
       <c r="F14" t="s">
-        <v>160</v>
+        <v>71</v>
       </c>
       <c r="G14">
         <v>0.2</v>
@@ -1613,13 +1670,13 @@
         <v>0.65</v>
       </c>
       <c r="J14" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="K14" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="L14" t="s">
-        <v>162</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
@@ -1630,7 +1687,7 @@
         <v>60</v>
       </c>
       <c r="C15" t="s">
-        <v>165</v>
+        <v>76</v>
       </c>
       <c r="D15">
         <v>19545</v>
@@ -1639,7 +1696,7 @@
         <v>41000</v>
       </c>
       <c r="F15" t="s">
-        <v>160</v>
+        <v>71</v>
       </c>
       <c r="G15">
         <v>0.2</v>
@@ -1651,13 +1708,13 @@
         <v>0.65</v>
       </c>
       <c r="J15" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="K15" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="L15" t="s">
-        <v>162</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
@@ -1668,7 +1725,7 @@
         <v>115</v>
       </c>
       <c r="C16" t="s">
-        <v>166</v>
+        <v>77</v>
       </c>
       <c r="D16">
         <v>11679</v>
@@ -1677,7 +1734,7 @@
         <v>27445</v>
       </c>
       <c r="F16" t="s">
-        <v>160</v>
+        <v>71</v>
       </c>
       <c r="G16">
         <v>0.2</v>
@@ -1689,13 +1746,13 @@
         <v>0.6</v>
       </c>
       <c r="J16" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="K16" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="L16" t="s">
-        <v>162</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
@@ -1706,7 +1763,7 @@
         <v>116</v>
       </c>
       <c r="C17" t="s">
-        <v>166</v>
+        <v>77</v>
       </c>
       <c r="D17">
         <v>11679</v>
@@ -1715,7 +1772,7 @@
         <v>27445</v>
       </c>
       <c r="F17" t="s">
-        <v>160</v>
+        <v>71</v>
       </c>
       <c r="G17">
         <v>0.2</v>
@@ -1727,13 +1784,13 @@
         <v>0.6</v>
       </c>
       <c r="J17" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="K17" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="L17" t="s">
-        <v>162</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
@@ -1744,7 +1801,7 @@
         <v>117</v>
       </c>
       <c r="C18" t="s">
-        <v>166</v>
+        <v>77</v>
       </c>
       <c r="D18">
         <v>11679</v>
@@ -1753,7 +1810,7 @@
         <v>27445</v>
       </c>
       <c r="F18" t="s">
-        <v>160</v>
+        <v>71</v>
       </c>
       <c r="G18">
         <v>0.2</v>
@@ -1765,13 +1822,13 @@
         <v>0.6</v>
       </c>
       <c r="J18" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="K18" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="L18" t="s">
-        <v>162</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
@@ -1782,7 +1839,7 @@
         <v>118</v>
       </c>
       <c r="C19" t="s">
-        <v>166</v>
+        <v>77</v>
       </c>
       <c r="D19">
         <v>11679</v>
@@ -1791,7 +1848,7 @@
         <v>27445</v>
       </c>
       <c r="F19" t="s">
-        <v>160</v>
+        <v>71</v>
       </c>
       <c r="G19">
         <v>0.2</v>
@@ -1803,13 +1860,13 @@
         <v>0.6</v>
       </c>
       <c r="J19" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="K19" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="L19" t="s">
-        <v>162</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
@@ -1820,7 +1877,7 @@
         <v>131</v>
       </c>
       <c r="C20" t="s">
-        <v>167</v>
+        <v>78</v>
       </c>
       <c r="D20">
         <v>7875</v>
@@ -1829,16 +1886,16 @@
         <v>10500</v>
       </c>
       <c r="F20" t="s">
-        <v>168</v>
+        <v>79</v>
       </c>
       <c r="G20">
         <v>0.2</v>
       </c>
       <c r="H20" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="I20" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="J20">
         <v>6300</v>
@@ -1847,7 +1904,7 @@
         <v>15800</v>
       </c>
       <c r="L20" t="s">
-        <v>169</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
@@ -1858,7 +1915,7 @@
         <v>132</v>
       </c>
       <c r="C21" t="s">
-        <v>167</v>
+        <v>78</v>
       </c>
       <c r="D21">
         <v>7875</v>
@@ -1867,16 +1924,16 @@
         <v>10500</v>
       </c>
       <c r="F21" t="s">
-        <v>168</v>
+        <v>79</v>
       </c>
       <c r="G21">
         <v>0.2</v>
       </c>
       <c r="H21" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="I21" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="J21">
         <v>6300</v>
@@ -1885,7 +1942,7 @@
         <v>15800</v>
       </c>
       <c r="L21" t="s">
-        <v>169</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
@@ -1896,7 +1953,7 @@
         <v>135</v>
       </c>
       <c r="C22" t="s">
-        <v>170</v>
+        <v>81</v>
       </c>
       <c r="D22">
         <v>2500</v>
@@ -1905,16 +1962,16 @@
         <v>3333</v>
       </c>
       <c r="F22" t="s">
-        <v>168</v>
+        <v>79</v>
       </c>
       <c r="G22">
         <v>0.2</v>
       </c>
       <c r="H22" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="I22" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="J22">
         <v>2000</v>
@@ -1923,7 +1980,7 @@
         <v>5000</v>
       </c>
       <c r="L22" t="s">
-        <v>169</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
@@ -1934,7 +1991,7 @@
         <v>136</v>
       </c>
       <c r="C23" t="s">
-        <v>170</v>
+        <v>81</v>
       </c>
       <c r="D23">
         <v>2500</v>
@@ -1943,16 +2000,16 @@
         <v>3333</v>
       </c>
       <c r="F23" t="s">
-        <v>168</v>
+        <v>79</v>
       </c>
       <c r="G23">
         <v>0.2</v>
       </c>
       <c r="H23" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="I23" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="J23">
         <v>2000</v>
@@ -1961,7 +2018,7 @@
         <v>5000</v>
       </c>
       <c r="L23" t="s">
-        <v>169</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
@@ -1972,7 +2029,7 @@
         <v>139</v>
       </c>
       <c r="C24" t="s">
-        <v>171</v>
+        <v>82</v>
       </c>
       <c r="D24">
         <v>7250</v>
@@ -1981,16 +2038,16 @@
         <v>9667</v>
       </c>
       <c r="F24" t="s">
-        <v>168</v>
+        <v>79</v>
       </c>
       <c r="G24">
         <v>0.2</v>
       </c>
       <c r="H24" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="I24" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="J24">
         <v>5800</v>
@@ -1999,7 +2056,7 @@
         <v>14500</v>
       </c>
       <c r="L24" t="s">
-        <v>169</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
@@ -2010,7 +2067,7 @@
         <v>140</v>
       </c>
       <c r="C25" t="s">
-        <v>171</v>
+        <v>82</v>
       </c>
       <c r="D25">
         <v>7250</v>
@@ -2019,16 +2076,16 @@
         <v>9667</v>
       </c>
       <c r="F25" t="s">
-        <v>168</v>
+        <v>79</v>
       </c>
       <c r="G25">
         <v>0.2</v>
       </c>
       <c r="H25" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="I25" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="J25">
         <v>5800</v>
@@ -2037,7 +2094,7 @@
         <v>14500</v>
       </c>
       <c r="L25" t="s">
-        <v>169</v>
+        <v>80</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
@@ -2048,7 +2105,7 @@
         <v>149</v>
       </c>
       <c r="C26" t="s">
-        <v>172</v>
+        <v>83</v>
       </c>
       <c r="D26">
         <v>44250</v>
@@ -2057,13 +2114,13 @@
         <v>59000</v>
       </c>
       <c r="F26" t="s">
-        <v>168</v>
+        <v>79</v>
       </c>
       <c r="G26" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="H26" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="I26">
         <v>0.6</v>
@@ -2075,7 +2132,7 @@
         <v>35400</v>
       </c>
       <c r="L26" t="s">
-        <v>169</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
@@ -2086,7 +2143,7 @@
         <v>150</v>
       </c>
       <c r="C27" t="s">
-        <v>172</v>
+        <v>83</v>
       </c>
       <c r="D27">
         <v>44250</v>
@@ -2095,13 +2152,13 @@
         <v>59000</v>
       </c>
       <c r="F27" t="s">
-        <v>168</v>
+        <v>79</v>
       </c>
       <c r="G27" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="H27" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="I27">
         <v>0.6</v>
@@ -2113,7 +2170,7 @@
         <v>35400</v>
       </c>
       <c r="L27" t="s">
-        <v>169</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
@@ -2124,7 +2181,7 @@
         <v>153</v>
       </c>
       <c r="C28" t="s">
-        <v>172</v>
+        <v>83</v>
       </c>
       <c r="D28">
         <v>44250</v>
@@ -2133,13 +2190,13 @@
         <v>59000</v>
       </c>
       <c r="F28" t="s">
-        <v>168</v>
+        <v>79</v>
       </c>
       <c r="G28" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="H28" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="I28">
         <v>0.6</v>
@@ -2151,7 +2208,7 @@
         <v>35400</v>
       </c>
       <c r="L28" t="s">
-        <v>169</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
@@ -2162,7 +2219,7 @@
         <v>154</v>
       </c>
       <c r="C29" t="s">
-        <v>172</v>
+        <v>83</v>
       </c>
       <c r="D29">
         <v>44250</v>
@@ -2171,13 +2228,13 @@
         <v>59000</v>
       </c>
       <c r="F29" t="s">
-        <v>168</v>
+        <v>79</v>
       </c>
       <c r="G29" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="H29" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="I29">
         <v>0.6</v>
@@ -2189,7 +2246,7 @@
         <v>35400</v>
       </c>
       <c r="L29" t="s">
-        <v>169</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
@@ -2200,7 +2257,7 @@
         <v>157</v>
       </c>
       <c r="C30" t="s">
-        <v>172</v>
+        <v>83</v>
       </c>
       <c r="D30">
         <v>44250</v>
@@ -2209,13 +2266,13 @@
         <v>59000</v>
       </c>
       <c r="F30" t="s">
-        <v>168</v>
+        <v>79</v>
       </c>
       <c r="G30" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="H30" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="I30">
         <v>0.6</v>
@@ -2227,7 +2284,7 @@
         <v>35400</v>
       </c>
       <c r="L30" t="s">
-        <v>169</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
@@ -2238,7 +2295,7 @@
         <v>158</v>
       </c>
       <c r="C31" t="s">
-        <v>172</v>
+        <v>83</v>
       </c>
       <c r="D31">
         <v>44250</v>
@@ -2247,13 +2304,13 @@
         <v>59000</v>
       </c>
       <c r="F31" t="s">
-        <v>168</v>
+        <v>79</v>
       </c>
       <c r="G31" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="H31" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="I31">
         <v>0.6</v>
@@ -2265,7 +2322,7 @@
         <v>35400</v>
       </c>
       <c r="L31" t="s">
-        <v>169</v>
+        <v>80</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
@@ -2276,34 +2333,34 @@
         <v>227</v>
       </c>
       <c r="C32" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D32" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="E32" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="F32" t="s">
-        <v>183</v>
+        <v>94</v>
       </c>
       <c r="G32" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="H32" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="I32" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="J32" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="K32" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="L32" t="s">
-        <v>173</v>
+        <v>84</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
@@ -2314,34 +2371,34 @@
         <v>228</v>
       </c>
       <c r="C33" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D33" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="E33" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="F33" t="s">
-        <v>183</v>
+        <v>94</v>
       </c>
       <c r="G33" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="H33" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="I33" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="J33" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="K33" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="L33" t="s">
-        <v>173</v>
+        <v>84</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
@@ -2352,34 +2409,34 @@
         <v>231</v>
       </c>
       <c r="C34" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D34" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="E34" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="F34" t="s">
-        <v>174</v>
+        <v>85</v>
       </c>
       <c r="G34">
         <v>0.2</v>
       </c>
       <c r="H34" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="I34" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="J34" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="K34" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="L34" t="s">
-        <v>175</v>
+        <v>86</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
@@ -2390,34 +2447,34 @@
         <v>232</v>
       </c>
       <c r="C35" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D35" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="E35" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="F35" t="s">
-        <v>174</v>
+        <v>85</v>
       </c>
       <c r="G35">
         <v>0.2</v>
       </c>
       <c r="H35" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="I35" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="J35" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="K35" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="L35" t="s">
-        <v>175</v>
+        <v>86</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
@@ -2428,34 +2485,34 @@
         <v>207</v>
       </c>
       <c r="C36" t="s">
-        <v>176</v>
+        <v>87</v>
       </c>
       <c r="D36" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="E36" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="F36" t="s">
-        <v>183</v>
+        <v>94</v>
       </c>
       <c r="G36" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="H36" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="I36" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="J36" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="K36" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="L36" t="s">
-        <v>173</v>
+        <v>84</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
@@ -2466,34 +2523,34 @@
         <v>208</v>
       </c>
       <c r="C37" t="s">
-        <v>176</v>
+        <v>87</v>
       </c>
       <c r="D37" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="E37" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="F37" t="s">
-        <v>183</v>
+        <v>94</v>
       </c>
       <c r="G37" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="H37" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="I37" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="J37" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="K37" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="L37" t="s">
-        <v>173</v>
+        <v>84</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
@@ -2504,34 +2561,34 @@
         <v>211</v>
       </c>
       <c r="C38" t="s">
-        <v>177</v>
+        <v>88</v>
       </c>
       <c r="D38" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="E38" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="F38" t="s">
-        <v>183</v>
+        <v>94</v>
       </c>
       <c r="G38" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="H38" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="I38" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="J38" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="K38" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="L38" t="s">
-        <v>173</v>
+        <v>84</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
@@ -2542,34 +2599,34 @@
         <v>212</v>
       </c>
       <c r="C39" t="s">
-        <v>177</v>
+        <v>88</v>
       </c>
       <c r="D39" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="E39" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="F39" t="s">
-        <v>183</v>
+        <v>94</v>
       </c>
       <c r="G39" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="H39" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="I39" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="J39" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="K39" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="L39" t="s">
-        <v>173</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -2779,82 +2836,82 @@
     </row>
     <row r="2" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="9"/>
       <c r="B3" s="9" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="8"/>
       <c r="B4" s="8" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="9"/>
       <c r="B5" s="9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="8"/>
       <c r="B7" s="8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="9"/>
       <c r="B8" s="9" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="8"/>
       <c r="B9" s="8" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="9"/>
       <c r="B10" s="9" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="8"/>
       <c r="B12" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="8" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -2865,445 +2922,435 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="103.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.77734375" customWidth="1"/>
+    <col min="2" max="2" width="40.6640625" style="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" t="s">
-        <v>37</v>
+        <v>101</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>102</v>
       </c>
       <c r="C1" t="s">
-        <v>35</v>
+        <v>165</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B2" t="s">
-        <v>55</v>
+        <v>109</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C3" t="s">
-        <v>35</v>
+        <v>110</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>58</v>
-      </c>
-      <c r="B4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C4" t="s">
-        <v>39</v>
+        <v>111</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B5" t="s">
-        <v>61</v>
+        <v>185</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>135</v>
       </c>
       <c r="C5" t="s">
-        <v>62</v>
+        <v>166</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>63</v>
-      </c>
-      <c r="B6" t="s">
-        <v>64</v>
+        <v>186</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>136</v>
       </c>
       <c r="C6" t="s">
-        <v>62</v>
+        <v>167</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>65</v>
-      </c>
-      <c r="B7" t="s">
-        <v>66</v>
+        <v>112</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>67</v>
-      </c>
-      <c r="B8" t="s">
-        <v>68</v>
+        <v>113</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>69</v>
-      </c>
-      <c r="B9" t="s">
-        <v>70</v>
-      </c>
-      <c r="C9" t="s">
-        <v>62</v>
+        <v>114</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>71</v>
-      </c>
-      <c r="B10" t="s">
-        <v>72</v>
-      </c>
-      <c r="C10" t="s">
-        <v>35</v>
+        <v>115</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>73</v>
-      </c>
-      <c r="B11" t="s">
-        <v>74</v>
-      </c>
-      <c r="C11" t="s">
-        <v>35</v>
+        <v>116</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>75</v>
+        <v>187</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>140</v>
       </c>
       <c r="C12" t="s">
-        <v>76</v>
+        <v>168</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>77</v>
+        <v>188</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>141</v>
       </c>
       <c r="C13" t="s">
-        <v>78</v>
+        <v>169</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>79</v>
-      </c>
-      <c r="B14" t="s">
-        <v>80</v>
+        <v>117</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>142</v>
       </c>
       <c r="C14" t="s">
-        <v>35</v>
+        <v>204</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>81</v>
-      </c>
-      <c r="B15" t="s">
-        <v>82</v>
-      </c>
-      <c r="C15" t="s">
-        <v>35</v>
+        <v>118</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>156</v>
-      </c>
-      <c r="B16" t="s">
-        <v>157</v>
+        <v>67</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>83</v>
-      </c>
-      <c r="B17" t="s">
-        <v>84</v>
+        <v>119</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>85</v>
-      </c>
-      <c r="C18" t="s">
-        <v>86</v>
+        <v>120</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>87</v>
-      </c>
-      <c r="B19" t="s">
-        <v>88</v>
-      </c>
-      <c r="C19" t="s">
-        <v>35</v>
+        <v>121</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>89</v>
-      </c>
-      <c r="B20" t="s">
-        <v>90</v>
-      </c>
-      <c r="C20" t="s">
-        <v>35</v>
+        <v>122</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>91</v>
-      </c>
-      <c r="B21" t="s">
-        <v>92</v>
+        <v>189</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="C21" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>93</v>
-      </c>
-      <c r="B22" t="s">
-        <v>94</v>
-      </c>
-      <c r="C22" t="s">
-        <v>62</v>
+        <v>123</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>95</v>
-      </c>
-      <c r="B23" t="s">
-        <v>96</v>
+        <v>190</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>146</v>
       </c>
       <c r="C23" t="s">
-        <v>62</v>
+        <v>171</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>97</v>
-      </c>
-      <c r="B24" t="s">
-        <v>98</v>
+        <v>191</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="C24" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>99</v>
-      </c>
-      <c r="B25" t="s">
-        <v>100</v>
+        <v>192</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="C25" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>101</v>
-      </c>
-      <c r="B26" t="s">
-        <v>102</v>
-      </c>
-      <c r="C26" t="s">
-        <v>35</v>
+        <v>124</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>103</v>
-      </c>
-      <c r="B27" t="s">
-        <v>104</v>
-      </c>
-      <c r="C27" t="s">
-        <v>62</v>
+        <v>125</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>105</v>
+        <v>193</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>174</v>
       </c>
       <c r="C28" t="s">
-        <v>106</v>
+        <v>175</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>107</v>
-      </c>
-      <c r="B29" t="s">
-        <v>108</v>
-      </c>
-      <c r="C29" t="s">
-        <v>35</v>
+        <v>126</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>109</v>
-      </c>
-      <c r="B30" t="s">
-        <v>110</v>
+        <v>194</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>152</v>
       </c>
       <c r="C30" t="s">
-        <v>35</v>
+        <v>176</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>111</v>
-      </c>
-      <c r="B31" t="s">
-        <v>112</v>
+        <v>195</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>107</v>
       </c>
       <c r="C31" t="s">
-        <v>35</v>
+        <v>177</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>113</v>
-      </c>
-      <c r="B32" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+        <v>196</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="C32" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>115</v>
-      </c>
-      <c r="B33" t="s">
-        <v>116</v>
+        <v>197</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>154</v>
       </c>
       <c r="C33" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>117</v>
-      </c>
-      <c r="B34" t="s">
-        <v>62</v>
+        <v>198</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>155</v>
       </c>
       <c r="C34" t="s">
-        <v>118</v>
-      </c>
-      <c r="D34" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>119</v>
-      </c>
-      <c r="C35" t="s">
-        <v>120</v>
-      </c>
-      <c r="D35" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>121</v>
-      </c>
-      <c r="C36" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+        <v>128</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>123</v>
-      </c>
-      <c r="B37" t="s">
-        <v>124</v>
-      </c>
-      <c r="C37" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+        <v>129</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>125</v>
-      </c>
-      <c r="B38" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+        <v>199</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="C38" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>127</v>
-      </c>
-      <c r="B39" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+        <v>200</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="C39" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>129</v>
-      </c>
-      <c r="B40" t="s">
+        <v>201</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="C40" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+      <c r="B41" s="11" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>202</v>
+      </c>
+      <c r="B42" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="C42" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
         <v>131</v>
       </c>
-      <c r="B41" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>133</v>
-      </c>
-      <c r="B42" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>135</v>
-      </c>
-      <c r="B43" t="s">
-        <v>136</v>
-      </c>
-      <c r="C43" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B43" s="11" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>137</v>
-      </c>
-      <c r="B44" t="s">
-        <v>138</v>
+        <v>203</v>
+      </c>
+      <c r="B44" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="C44" t="s">
+        <v>184</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
integrating CCT pre-Feb 23 edits, mostly text
</commit_message>
<xml_diff>
--- a/StaticTables.xlsx
+++ b/StaticTables.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stateofwa-my.sharepoint.com/personal/daniel_auerbach_dfw_wa_gov/Documents/code/PeriodicReport/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doimspp-my.sharepoint.com/personal/carrie_cook-tabor_fws_gov/Documents/PSC Coho_cct/periodic report/2019 New Report/for dan to upload/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="121" documentId="13_ncr:1_{793868AE-9DA0-439D-B941-FC5A2F22A4BB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{8DB362CD-B9FC-4018-A61F-EA166A48FCF3}"/>
   <bookViews>
-    <workbookView xWindow="-15410" yWindow="-19670" windowWidth="33330" windowHeight="16960" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18540" windowHeight="1860" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="members" sheetId="5" r:id="rId1"/>
@@ -18,8 +17,11 @@
     <sheet name="RunFiles" sheetId="1" r:id="rId3"/>
     <sheet name="CUs" sheetId="2" r:id="rId4"/>
     <sheet name="acronyms" sheetId="3" r:id="rId5"/>
+    <sheet name="glossary" sheetId="9" r:id="rId6"/>
+    <sheet name="Readme" sheetId="8" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="324">
   <si>
     <t>BK04.Cmd</t>
   </si>
@@ -184,9 +186,6 @@
     <t>Howe Sound – Burrard Inlet</t>
   </si>
   <si>
-    <t>Georgia Strait Vancouver Island</t>
-  </si>
-  <si>
     <t>East Vancouver Island – Georgia Strait</t>
   </si>
   <si>
@@ -211,12 +210,6 @@
     <t>Ms. Carrie Cook-Tabor, USFWS</t>
   </si>
   <si>
-    <t>Mr. Roger Dunlop, NTC</t>
-  </si>
-  <si>
-    <t>Ms. Marlene Bellman, NWIFC</t>
-  </si>
-  <si>
     <t>Mr. Michael Arbeider, CDFO</t>
   </si>
   <si>
@@ -235,9 +228,6 @@
     <t>Dr. Daniel Auerbach, WDFW</t>
   </si>
   <si>
-    <t>Ms. Christine Mallette, ODFW</t>
-  </si>
-  <si>
     <t>Ms. Ashlee Prevost, LFFA</t>
   </si>
   <si>
@@ -653,13 +643,384 @@
   </si>
   <si>
     <t>https://framverse.github.io/fram_doc/</t>
+  </si>
+  <si>
+    <t>Mr. Kristopher Hein, CDFO</t>
+  </si>
+  <si>
+    <t>Ms. Cassandra R. Leeman, ODFW</t>
+  </si>
+  <si>
+    <t>Ms. Madeline Thomson, CDFO</t>
+  </si>
+  <si>
+    <t>Mr. Kevin Pellet, CDFO</t>
+  </si>
+  <si>
+    <t>Mr. Roger Dunlop, MMFN</t>
+  </si>
+  <si>
+    <t>MMFN</t>
+  </si>
+  <si>
+    <t>Mowachaht-Muchalaht First Nation</t>
+  </si>
+  <si>
+    <t>https://www.yuquot.ca/</t>
+  </si>
+  <si>
+    <t>Georgia Strait (Mainland and Vancouver Island)</t>
+  </si>
+  <si>
+    <t>changes made:</t>
+  </si>
+  <si>
+    <t>last updated</t>
+  </si>
+  <si>
+    <t>changed organization for Roger Dunlop</t>
+  </si>
+  <si>
+    <t>added MMFN to acronym:</t>
+  </si>
+  <si>
+    <t>Date:</t>
+  </si>
+  <si>
+    <t>updated CoTC member list to include everyone currently on the CoTC membership list on the PSC website</t>
+  </si>
+  <si>
+    <t>on CUs tab combine georgia strait MUs</t>
+  </si>
+  <si>
+    <t>mainland and vancouver island MUs combined for list of conservation units</t>
+  </si>
+  <si>
+    <t>NEED</t>
+  </si>
+  <si>
+    <t>a full list of runfiles through pre-season 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Pacific Salmon Commission is an international organization, governed by the Pacific Salmon Treaty, and is a decision-making body for cooperative management of Pacific salmon between the U.S. and Canada. </t>
+  </si>
+  <si>
+    <t>The Pacific Salmon Treaty is a mutual international agreement and cooperative fishery management process formed between the governments of the United States and Canada. The Treaty regulates the fisheries that occur in the ocean and inland waters of Oregon, Washington, British Columbia, the Yukon, and southeast Alaska, and includes the rivers that flow into these waters.</t>
+  </si>
+  <si>
+    <t>Maximum Fishing Mortality Threshold</t>
+  </si>
+  <si>
+    <t>MFMT</t>
+  </si>
+  <si>
+    <t>IFMP</t>
+  </si>
+  <si>
+    <t>Integrated Fisheries Management Plan</t>
+  </si>
+  <si>
+    <t>FMP</t>
+  </si>
+  <si>
+    <t>Fisheries Management Plan</t>
+  </si>
+  <si>
+    <t>added more acronyms</t>
+  </si>
+  <si>
+    <t>Term</t>
+  </si>
+  <si>
+    <t>Co-management</t>
+  </si>
+  <si>
+    <t>The Endangered Species Act (ESA) is the primary law in the United States for protecting critically important species that are at risk of extinction. Under the ESA, the federal government has the responsibility to protect these species and their critical habitats. NOAA Fisheries is responsible for endangered and threatened salmon.</t>
+  </si>
+  <si>
+    <t>Catch</t>
+  </si>
+  <si>
+    <t>Exclusive Economic Zone</t>
+  </si>
+  <si>
+    <t>The Exclusive Economic Zone (EEZ) is an area from 3 to 200 nautical miles offshore of coastal states and is classified as federal waters. In the EEZ, the U.S. has special rights about the exploration and use of marine resources, which includes energy production from water and wind, and fisheries.</t>
+  </si>
+  <si>
+    <t>Fisheries management is a process that relies on science, management approaches, enforcement, partnerships, and public participation. Fisheries management uses scientific information (e.g., number of fish caught, types of fish caught, life cycle knowledge) and input from fishing communities to help guide management decisions and conservation objectives.</t>
+  </si>
+  <si>
+    <t>Fisheries Management</t>
+  </si>
+  <si>
+    <t>The term harvest refers to the total number of fish caught and kept from an area or fishery during a period of time.</t>
+  </si>
+  <si>
+    <t>Harvest</t>
+  </si>
+  <si>
+    <t>A fishery is an activity leading to the harvesting of fish and can be specified by the species of fish caught, people involved, location, method of fishing, and purpose of the activities. Fish caught in a fishery can be for commercial, recreational, or tribal and ceremonial purposes.
+Harvest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fishery </t>
+  </si>
+  <si>
+    <t>Interception</t>
+  </si>
+  <si>
+    <t>Interception occurs when a salmon from one state or country is caught in another state or country's fisheries. As salmon grow and mature in the Pacific Ocean, they travel along the West Coast and across international borders. Salmon that are born in U.S. streams may migrate through Canadian waters, where they may be caught in Canadian fisheries. Salmon from Oregon streams can be caught in Washington fisheries.</t>
+  </si>
+  <si>
+    <t>Magnuson-Stevens Fishery Conservation and Management Act (MSA)</t>
+  </si>
+  <si>
+    <t>The Magnuson-Stevens Fishery Conservation and Management Act (MSA) is the primary law that governs fisheries management in the federal marine waters (3-200 miles offshore) of the United States. The goal of the MSA is to encourage the long-term biological and economic sustainability of marine fisheries.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Database containing data on salmonid releases, recoveries in fisheries and escapement, and estimated catch by fishery and time period.  </t>
+  </si>
+  <si>
+    <t>Run</t>
+  </si>
+  <si>
+    <t>As salmon migrate back to freshwater as adults, they arrive in groups called runs, which are typically associated with a season (spring, summer, fall, winter). A run of salmon may be composed of salmon from a single age or multiple ages, and can be from a single stock or multiple stocks.</t>
+  </si>
+  <si>
+    <t>Spawning grounds/Spawn</t>
+  </si>
+  <si>
+    <t>Subsistence Fisheries</t>
+  </si>
+  <si>
+    <t>In the Pacific Northwest of the U.S., the term "Ceremonial and Subsistence" (C&amp;S) is used to describe non-commercial harvest in Treaty Tribe fisheries for personal, ritual, or community use. In Canada, the term "Food, Social, and Ceremonial" (FSC) is used to describe the non-commercial harvest of fish by the First Nations.</t>
+  </si>
+  <si>
+    <t>Treaty/Treaties</t>
+  </si>
+  <si>
+    <t>Pacific States Marine Fisheries Commission (PSMFC) is a non‐regulatory agency that serves Alaska, California, Idaho, Oregon, and Washington. PSMFC (headquartered in Portland) administers salmon disaster relief funds, provides a communication exchange between the Pacific Fishery Management Council and the North Pacific Fishery Management Council, and provides information in the form of data services for various fisheries.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pacific States Marine Fisheries Commission </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The process of rebuilding an overfished stock. For salmon, rebuilding usually takes the form of reduced
+harvest limits. </t>
+  </si>
+  <si>
+    <t>Rebuilding</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>The year in which the majority of the parents of the fish spawned.</t>
+  </si>
+  <si>
+    <t>The number of fish that are caught in a fishery.</t>
+  </si>
+  <si>
+    <t>The collaborative process between co-managers–tribal governments and state governments on the West Coast. Using scientific information, the co-managers make decisions about the management of fisheries to ensure that the fisheries meet legal requirements, treaty fishing rights, and conservation goals.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A distinctive group of Pacific salmon, steelhead, or sea‐run cutthroat trout that is uniquely adapted to a particular area or environment and cannot be replaced. </t>
+  </si>
+  <si>
+    <t>By-catch</t>
+  </si>
+  <si>
+    <t>Incidental or unintentional catch of non-target stocks or species.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enhancement </t>
+  </si>
+  <si>
+    <t>Use of hatcheries, spawning channels, lake fertilization or habitat restoration to increase the survival rate or production of salmon at some stage of its life.</t>
+  </si>
+  <si>
+    <t>Endangered Species Act  (U.S.)</t>
+  </si>
+  <si>
+    <t>Expressed as a percentage, the proportion of the total return of adult salmon in a given year that die as a result of fishing activity.</t>
+  </si>
+  <si>
+    <t>Fry</t>
+  </si>
+  <si>
+    <t>Salmon that have emerged from gravel, completed yolk absorption, remained in freshwater streams, and are less than a few months old.</t>
+  </si>
+  <si>
+    <t>First Nations' fishery for food, social and ceremonial use. See "communal licence" above.</t>
+  </si>
+  <si>
+    <t>FSC (Canada)</t>
+  </si>
+  <si>
+    <t>Identify the main objectives and requirements for Pacific fisheries and outline the management to achieve these objectives. IFMPs provide a common understanding of the basic rules for the sustainable management of the fisheries resource, and communicate basic information about fish stocks and our fisheries.</t>
+  </si>
+  <si>
+    <t>https://www.pac.dfo-mpo.gc.ca/fm-gp/ifmp-eng.html#Salmon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">added a glossary of terms </t>
+  </si>
+  <si>
+    <t>located most info on PFMC, CDFO, and ADFG websites</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An estimate of the largest average annual catch or yield that can be continuously taken over a long period from a stock under prevailing ecological and environmental conditions.  </t>
+  </si>
+  <si>
+    <t>Stock</t>
+  </si>
+  <si>
+    <t>Pacific Salmon Commission (PSC)</t>
+  </si>
+  <si>
+    <t>A joint Canada/U.S. commission established under the Pacific Salmon Treaty to oversee the implementation of the Pacific Salmon Treaty.</t>
+  </si>
+  <si>
+    <t>Pacific Salmon Treaty (PST)</t>
+  </si>
+  <si>
+    <t>A treaty between Canada and the United States concerning the conservation, management, restoration, and enhancement of pacific salmon resources.</t>
+  </si>
+  <si>
+    <t>Southern Coho Management Plan (SCMP)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An agreement between the U.S. and Canada that specifies how the Parties’ fisheries impact on Coho Salmon that originate in southern British Columbia, Washington and Oregon shall be managed, subject to future approved technical refinements.   It is described in Annex IV, Chapter 5 of the current Pacific Salmon Treaty. </t>
+  </si>
+  <si>
+    <t>SCMP</t>
+  </si>
+  <si>
+    <t>Southern Coho Management Plan</t>
+  </si>
+  <si>
+    <t>Smolt</t>
+  </si>
+  <si>
+    <t>A smolt is a life cycle phase of a salmon or steelhead when the fish is preparing for the transition from freshwater to saltwater. The process is called smoltification. A smolt becomes physiologically capable of balancing salt and water in the estuary and ocean waters. Smolts vary in size and age depending on the species of salmon.</t>
+  </si>
+  <si>
+    <t>Spawning grounds are the freshwater areas where salmon and steelhead spawn. When Pacific salmon and steelhead spawn, females create nests (called “redds”) in the gravel where they lay thousands of eggs, which are then fertilized by males. Salmon and steelhead travel great distances to reach their spawning grounds in rivers and streams.</t>
+  </si>
+  <si>
+    <t>A treaty is a formal, legally binding agreement that establishes obligations between and among two or more countries, states, or sovereign nations. Examples of treaties include the Pacific Salmon Treaty and treaties between the U.S. and American Indian Tribes.</t>
+  </si>
+  <si>
+    <t>In all species of Pacific salmon but pinks, the individual salmon produced in any one spawning year mature and return to spawn in more than one subsequent year. All of the fish that return from a spawning year (the brood year) are collectively referred to as a cohort or the brood-year return. A sibling forecast uses the first returns from a cohort to predict the number of their siblings that will return in subsequent years. Generally, the first year of return is dominated by males and the last year of returns by females.</t>
+  </si>
+  <si>
+    <t>Sibling Forecast</t>
+  </si>
+  <si>
+    <t>Mark-Selective Fisheries</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A fisheries management approach which allows retention of hatchery marked fish, while requiring wild unmarked fish to be released unharmed. </t>
+  </si>
+  <si>
+    <t>A small piece of magnetized stainless steel wire that is injected into the snout of a juvenile salmon (usually hatchery stock). Each tag is 0.25 mm in diamter and typically 1.1 mm long and is etched with a code that identifies its release group.  Information on the release group is stored in the Regional Mark Information System's Release database under the tag code.</t>
+  </si>
+  <si>
+    <t>Double-Index Tag (DIT)</t>
+  </si>
+  <si>
+    <t>Coded-Wire Tag (CWT)</t>
+  </si>
+  <si>
+    <t>Conservation Unit (CU)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A double-index-tag group includes two coded-wire-tag (CWT) paired-release groups, one marked and one unmarked.  </t>
+  </si>
+  <si>
+    <t>Single Index Tag (SIT)</t>
+  </si>
+  <si>
+    <t>A group of coded-wire-tagged (CWT) fish that are not paired with another release group.  They can be marked (clipped) or unmarked (unclipped).</t>
+  </si>
+  <si>
+    <t>Escapement (Spawning Escapement)</t>
+  </si>
+  <si>
+    <t>The number of adult salmon that escape all fisheries and other forms of mortality to return to a hatchery or stream to spawn.</t>
+  </si>
+  <si>
+    <t>A group of interbreeding organisms that is relatively isolated (i.e. demographically uncoupled) from other such groups and is likely adapted to the local habitat.  Fish species are made up of an aggregate of stocks.</t>
+  </si>
+  <si>
+    <t>Stock Assessment</t>
+  </si>
+  <si>
+    <t>Cohort Reconstruction</t>
+  </si>
+  <si>
+    <t>Base Period (FRAM)</t>
+  </si>
+  <si>
+    <t>The use of various statistical and mathematical calculations to make quantitative predictions about the reactions of fish populations to alternative management choices.</t>
+  </si>
+  <si>
+    <t>Fishing with a hook or hooks attached to a line that is towed through the water or from a vessel. Commercial trollers employ hooks and lines that are suspended from large poles extending from the fishing vessel</t>
+  </si>
+  <si>
+    <t>Troll Fishery (Trolling)</t>
+  </si>
+  <si>
+    <t>WCVI</t>
+  </si>
+  <si>
+    <t>West Coast of Vancouver Island</t>
+  </si>
+  <si>
+    <t>Wild Salmon</t>
+  </si>
+  <si>
+    <t>Salmon are considered "wild" if they have spent their entire life cycle in the wild and originate from parents that were also produced by natural spawning and continuously lived in the wild.</t>
+  </si>
+  <si>
+    <t>The FRAM base period was developed by summarizing coded-wire-tag information from a continuous time period that contains a sufficient number of CWT releases and fishery recoveries. The Coho base period is comprised of CWT recoveries from catch years 1986–1992. The Mixed-stock Model (MSM) and cohort reconstuction methods were used to estimate base period exploitation rates and other parameters, such as base period cohort sizes and fishery compositions, for all FRAM stocks and fisheries by time step. The base period is made up of the averages  of these estimates over the catch years 1986 through 1992. Using these base period parameters allows FRAM to predict the stock composition, exploitation rates, and escapements of future fisheries when provided with forecasts of abundance and fishery mortalities.</t>
+  </si>
+  <si>
+    <t>Abundance-based management establishes harvest levels based on the status of the fish affected by the fishery. The purpose is to provide more protection when the status of the fish is low and the conservation need greatest, and more harvest opportunity when abundance is high</t>
+  </si>
+  <si>
+    <t>Fishery Regulation Assessment Model (FRAM)</t>
+  </si>
+  <si>
+    <t>Ocean Age-3 Abundance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Model used in pre-season to set salmon harvest levels and post-season (BkFRAM) to assess fishery impacts on adult fish.  It includes 246 stocks, 198 fisheries, and 5 time steps.  </t>
+  </si>
+  <si>
+    <t>BkFRAM</t>
+  </si>
+  <si>
+    <t>Backwards FRAM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pre-fishing age-3 abundance in the ocean after natural mortality has been subtracted. </t>
+  </si>
+  <si>
+    <t>Cohort Abundance</t>
+  </si>
+  <si>
+    <t>For each stock unit, an annual abundance is obtained from a regional expert, typically in the form of an ocean age-3 run size (pre-fishing age-3 abundance in the ocean after natural mortality has been subtracted). In a pre-season context these abundances come from annual forecasts, whereas in a post-season context the abundances are derived from estimates of actual returns. For Coho, an initial stock abundance is needed for adult fish (age-3) by mark status.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cohort reconstruction is a method commonly used in salmon stock assessment for estimation of exploitation rates. The basic principle of cohort reconstruction is the sequential estimation of a cohort’s abundance from the end of the cohort’s life span, when abundance is zero, to a speciﬁed earlier age (commonly age-3 for Coho). A full cohort reconstruction can becompleted only once the cohort’s life span has ended. Age-speciﬁc escapement and harvest data are required and, in general, the natural mortality rates are assumed. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -688,8 +1049,47 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -705,6 +1105,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF8F8F8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -732,28 +1150,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -764,6 +1164,67 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1044,148 +1505,154 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80E593F5-BCC8-42CF-BCE2-FAF93307032E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.42578125" customWidth="1"/>
+    <col min="2" max="2" width="33.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="B1" s="10" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>205</v>
+      </c>
+      <c r="B4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>201</v>
+      </c>
+      <c r="B5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>204</v>
+      </c>
+      <c r="B7" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>66</v>
-      </c>
-      <c r="B7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
-        <v>50</v>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>203</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FA2F8A4-2609-4EE6-A53A-ADC42F7FF467}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="14.5546875" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G1" t="s">
         <v>89</v>
       </c>
-      <c r="D1" t="s">
+      <c r="H1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I1" t="s">
         <v>92</v>
       </c>
-      <c r="E1" t="s">
-        <v>91</v>
-      </c>
-      <c r="F1" t="s">
-        <v>100</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>93</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
+        <v>94</v>
+      </c>
+      <c r="L1" t="s">
         <v>95</v>
       </c>
-      <c r="I1" t="s">
-        <v>96</v>
-      </c>
-      <c r="J1" t="s">
-        <v>97</v>
-      </c>
-      <c r="K1" t="s">
-        <v>98</v>
-      </c>
-      <c r="L1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1193,7 +1660,7 @@
         <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D2">
         <v>22857</v>
@@ -1202,7 +1669,7 @@
         <v>62500</v>
       </c>
       <c r="F2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G2">
         <v>0.2</v>
@@ -1214,16 +1681,16 @@
         <v>0.6</v>
       </c>
       <c r="J2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="K2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="L2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1231,7 +1698,7 @@
         <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D3">
         <v>22857</v>
@@ -1240,7 +1707,7 @@
         <v>62500</v>
       </c>
       <c r="F3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G3">
         <v>0.2</v>
@@ -1252,16 +1719,16 @@
         <v>0.6</v>
       </c>
       <c r="J3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="K3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="L3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1269,7 +1736,7 @@
         <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D4">
         <v>22857</v>
@@ -1278,7 +1745,7 @@
         <v>62500</v>
       </c>
       <c r="F4" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G4">
         <v>0.2</v>
@@ -1290,16 +1757,16 @@
         <v>0.6</v>
       </c>
       <c r="J4" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="K4" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="L4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1307,7 +1774,7 @@
         <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D5">
         <v>22857</v>
@@ -1316,7 +1783,7 @@
         <v>62500</v>
       </c>
       <c r="F5" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G5">
         <v>0.2</v>
@@ -1328,16 +1795,16 @@
         <v>0.6</v>
       </c>
       <c r="J5" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="K5" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="L5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1345,7 +1812,7 @@
         <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D6">
         <v>9385</v>
@@ -1354,7 +1821,7 @@
         <v>20000</v>
       </c>
       <c r="F6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G6">
         <v>0.2</v>
@@ -1366,16 +1833,16 @@
         <v>0.5</v>
       </c>
       <c r="J6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="K6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="L6" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2</v>
       </c>
@@ -1383,7 +1850,7 @@
         <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D7">
         <v>9385</v>
@@ -1392,7 +1859,7 @@
         <v>20000</v>
       </c>
       <c r="F7" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G7">
         <v>0.2</v>
@@ -1404,16 +1871,16 @@
         <v>0.5</v>
       </c>
       <c r="J7" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="K7" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="L7" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3</v>
       </c>
@@ -1421,7 +1888,7 @@
         <v>35</v>
       </c>
       <c r="C8" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D8">
         <v>51667</v>
@@ -1430,7 +1897,7 @@
         <v>125000</v>
       </c>
       <c r="F8" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G8">
         <v>0.2</v>
@@ -1442,16 +1909,16 @@
         <v>0.6</v>
       </c>
       <c r="J8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="K8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="L8" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3</v>
       </c>
@@ -1459,7 +1926,7 @@
         <v>36</v>
       </c>
       <c r="C9" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D9">
         <v>51667</v>
@@ -1468,7 +1935,7 @@
         <v>125000</v>
       </c>
       <c r="F9" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G9">
         <v>0.2</v>
@@ -1480,16 +1947,16 @@
         <v>0.6</v>
       </c>
       <c r="J9" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="K9" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="L9" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>4</v>
       </c>
@@ -1497,7 +1964,7 @@
         <v>45</v>
       </c>
       <c r="C10" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D10">
         <v>19545</v>
@@ -1506,7 +1973,7 @@
         <v>41000</v>
       </c>
       <c r="F10" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G10">
         <v>0.2</v>
@@ -1518,16 +1985,16 @@
         <v>0.65</v>
       </c>
       <c r="J10" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="K10" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="L10" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>4</v>
       </c>
@@ -1535,7 +2002,7 @@
         <v>46</v>
       </c>
       <c r="C11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D11">
         <v>19545</v>
@@ -1544,7 +2011,7 @@
         <v>41000</v>
       </c>
       <c r="F11" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G11">
         <v>0.2</v>
@@ -1556,16 +2023,16 @@
         <v>0.65</v>
       </c>
       <c r="J11" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="K11" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="L11" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>4</v>
       </c>
@@ -1573,7 +2040,7 @@
         <v>55</v>
       </c>
       <c r="C12" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D12">
         <v>19545</v>
@@ -1582,7 +2049,7 @@
         <v>41000</v>
       </c>
       <c r="F12" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G12">
         <v>0.2</v>
@@ -1594,16 +2061,16 @@
         <v>0.65</v>
       </c>
       <c r="J12" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="K12" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="L12" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>4</v>
       </c>
@@ -1611,7 +2078,7 @@
         <v>56</v>
       </c>
       <c r="C13" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D13">
         <v>19545</v>
@@ -1620,7 +2087,7 @@
         <v>41000</v>
       </c>
       <c r="F13" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G13">
         <v>0.2</v>
@@ -1632,16 +2099,16 @@
         <v>0.65</v>
       </c>
       <c r="J13" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="K13" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="L13" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>4</v>
       </c>
@@ -1649,7 +2116,7 @@
         <v>59</v>
       </c>
       <c r="C14" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D14">
         <v>19545</v>
@@ -1658,7 +2125,7 @@
         <v>41000</v>
       </c>
       <c r="F14" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G14">
         <v>0.2</v>
@@ -1670,16 +2137,16 @@
         <v>0.65</v>
       </c>
       <c r="J14" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="K14" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="L14" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>4</v>
       </c>
@@ -1687,7 +2154,7 @@
         <v>60</v>
       </c>
       <c r="C15" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D15">
         <v>19545</v>
@@ -1696,7 +2163,7 @@
         <v>41000</v>
       </c>
       <c r="F15" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G15">
         <v>0.2</v>
@@ -1708,16 +2175,16 @@
         <v>0.65</v>
       </c>
       <c r="J15" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="K15" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="L15" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>5</v>
       </c>
@@ -1725,7 +2192,7 @@
         <v>115</v>
       </c>
       <c r="C16" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D16">
         <v>11679</v>
@@ -1734,7 +2201,7 @@
         <v>27445</v>
       </c>
       <c r="F16" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G16">
         <v>0.2</v>
@@ -1746,16 +2213,16 @@
         <v>0.6</v>
       </c>
       <c r="J16" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="K16" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="L16" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>5</v>
       </c>
@@ -1763,7 +2230,7 @@
         <v>116</v>
       </c>
       <c r="C17" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D17">
         <v>11679</v>
@@ -1772,7 +2239,7 @@
         <v>27445</v>
       </c>
       <c r="F17" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G17">
         <v>0.2</v>
@@ -1784,16 +2251,16 @@
         <v>0.6</v>
       </c>
       <c r="J17" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="K17" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="L17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>5</v>
       </c>
@@ -1801,7 +2268,7 @@
         <v>117</v>
       </c>
       <c r="C18" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D18">
         <v>11679</v>
@@ -1810,7 +2277,7 @@
         <v>27445</v>
       </c>
       <c r="F18" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G18">
         <v>0.2</v>
@@ -1822,16 +2289,16 @@
         <v>0.6</v>
       </c>
       <c r="J18" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="K18" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="L18" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>5</v>
       </c>
@@ -1839,7 +2306,7 @@
         <v>118</v>
       </c>
       <c r="C19" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D19">
         <v>11679</v>
@@ -1848,7 +2315,7 @@
         <v>27445</v>
       </c>
       <c r="F19" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G19">
         <v>0.2</v>
@@ -1860,16 +2327,16 @@
         <v>0.6</v>
       </c>
       <c r="J19" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="K19" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="L19" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>6</v>
       </c>
@@ -1877,7 +2344,7 @@
         <v>131</v>
       </c>
       <c r="C20" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D20">
         <v>7875</v>
@@ -1886,16 +2353,16 @@
         <v>10500</v>
       </c>
       <c r="F20" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="G20">
         <v>0.2</v>
       </c>
       <c r="H20" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="I20" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="J20">
         <v>6300</v>
@@ -1904,10 +2371,10 @@
         <v>15800</v>
       </c>
       <c r="L20" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>6</v>
       </c>
@@ -1915,7 +2382,7 @@
         <v>132</v>
       </c>
       <c r="C21" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D21">
         <v>7875</v>
@@ -1924,16 +2391,16 @@
         <v>10500</v>
       </c>
       <c r="F21" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="G21">
         <v>0.2</v>
       </c>
       <c r="H21" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="I21" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="J21">
         <v>6300</v>
@@ -1942,10 +2409,10 @@
         <v>15800</v>
       </c>
       <c r="L21" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>7</v>
       </c>
@@ -1953,7 +2420,7 @@
         <v>135</v>
       </c>
       <c r="C22" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D22">
         <v>2500</v>
@@ -1962,16 +2429,16 @@
         <v>3333</v>
       </c>
       <c r="F22" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="G22">
         <v>0.2</v>
       </c>
       <c r="H22" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="I22" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="J22">
         <v>2000</v>
@@ -1980,10 +2447,10 @@
         <v>5000</v>
       </c>
       <c r="L22" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>7</v>
       </c>
@@ -1991,7 +2458,7 @@
         <v>136</v>
       </c>
       <c r="C23" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D23">
         <v>2500</v>
@@ -2000,16 +2467,16 @@
         <v>3333</v>
       </c>
       <c r="F23" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="G23">
         <v>0.2</v>
       </c>
       <c r="H23" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="I23" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="J23">
         <v>2000</v>
@@ -2018,10 +2485,10 @@
         <v>5000</v>
       </c>
       <c r="L23" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>8</v>
       </c>
@@ -2029,7 +2496,7 @@
         <v>139</v>
       </c>
       <c r="C24" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D24">
         <v>7250</v>
@@ -2038,16 +2505,16 @@
         <v>9667</v>
       </c>
       <c r="F24" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="G24">
         <v>0.2</v>
       </c>
       <c r="H24" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="I24" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="J24">
         <v>5800</v>
@@ -2056,10 +2523,10 @@
         <v>14500</v>
       </c>
       <c r="L24" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>8</v>
       </c>
@@ -2067,7 +2534,7 @@
         <v>140</v>
       </c>
       <c r="C25" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D25">
         <v>7250</v>
@@ -2076,16 +2543,16 @@
         <v>9667</v>
       </c>
       <c r="F25" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="G25">
         <v>0.2</v>
       </c>
       <c r="H25" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="I25" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="J25">
         <v>5800</v>
@@ -2094,10 +2561,10 @@
         <v>14500</v>
       </c>
       <c r="L25" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>9</v>
       </c>
@@ -2105,7 +2572,7 @@
         <v>149</v>
       </c>
       <c r="C26" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D26">
         <v>44250</v>
@@ -2114,13 +2581,13 @@
         <v>59000</v>
       </c>
       <c r="F26" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="G26" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="H26" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="I26">
         <v>0.6</v>
@@ -2132,10 +2599,10 @@
         <v>35400</v>
       </c>
       <c r="L26" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>9</v>
       </c>
@@ -2143,7 +2610,7 @@
         <v>150</v>
       </c>
       <c r="C27" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D27">
         <v>44250</v>
@@ -2152,13 +2619,13 @@
         <v>59000</v>
       </c>
       <c r="F27" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="G27" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="H27" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="I27">
         <v>0.6</v>
@@ -2170,10 +2637,10 @@
         <v>35400</v>
       </c>
       <c r="L27" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>9</v>
       </c>
@@ -2181,7 +2648,7 @@
         <v>153</v>
       </c>
       <c r="C28" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D28">
         <v>44250</v>
@@ -2190,13 +2657,13 @@
         <v>59000</v>
       </c>
       <c r="F28" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="G28" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="H28" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="I28">
         <v>0.6</v>
@@ -2208,10 +2675,10 @@
         <v>35400</v>
       </c>
       <c r="L28" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>9</v>
       </c>
@@ -2219,7 +2686,7 @@
         <v>154</v>
       </c>
       <c r="C29" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D29">
         <v>44250</v>
@@ -2228,13 +2695,13 @@
         <v>59000</v>
       </c>
       <c r="F29" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="G29" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="H29" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="I29">
         <v>0.6</v>
@@ -2246,10 +2713,10 @@
         <v>35400</v>
       </c>
       <c r="L29" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>9</v>
       </c>
@@ -2257,7 +2724,7 @@
         <v>157</v>
       </c>
       <c r="C30" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D30">
         <v>44250</v>
@@ -2266,13 +2733,13 @@
         <v>59000</v>
       </c>
       <c r="F30" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="G30" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="H30" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="I30">
         <v>0.6</v>
@@ -2284,10 +2751,10 @@
         <v>35400</v>
       </c>
       <c r="L30" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>9</v>
       </c>
@@ -2295,7 +2762,7 @@
         <v>158</v>
       </c>
       <c r="C31" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D31">
         <v>44250</v>
@@ -2304,13 +2771,13 @@
         <v>59000</v>
       </c>
       <c r="F31" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="G31" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="H31" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="I31">
         <v>0.6</v>
@@ -2322,10 +2789,10 @@
         <v>35400</v>
       </c>
       <c r="L31" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>10</v>
       </c>
@@ -2336,34 +2803,34 @@
         <v>36</v>
       </c>
       <c r="D32" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E32" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F32" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="G32" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="H32" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="I32" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="J32" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="K32" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="L32" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>10</v>
       </c>
@@ -2374,34 +2841,34 @@
         <v>36</v>
       </c>
       <c r="D33" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E33" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F33" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="G33" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="H33" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="I33" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="J33" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="K33" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="L33" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>11</v>
       </c>
@@ -2412,34 +2879,34 @@
         <v>40</v>
       </c>
       <c r="D34" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E34" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F34" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="G34">
         <v>0.2</v>
       </c>
       <c r="H34" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="I34" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="J34" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="K34" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="L34" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>11</v>
       </c>
@@ -2450,34 +2917,34 @@
         <v>40</v>
       </c>
       <c r="D35" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E35" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F35" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="G35">
         <v>0.2</v>
       </c>
       <c r="H35" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="I35" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="J35" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="K35" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="L35" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>12</v>
       </c>
@@ -2485,37 +2952,37 @@
         <v>207</v>
       </c>
       <c r="C36" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D36" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E36" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F36" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="G36" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="H36" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="I36" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="J36" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="K36" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="L36" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>12</v>
       </c>
@@ -2523,37 +2990,37 @@
         <v>208</v>
       </c>
       <c r="C37" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D37" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E37" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F37" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="G37" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="H37" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="I37" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="J37" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="K37" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="L37" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>13</v>
       </c>
@@ -2561,37 +3028,37 @@
         <v>211</v>
       </c>
       <c r="C38" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D38" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E38" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F38" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="G38" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="H38" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="I38" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="J38" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="K38" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="L38" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>13</v>
       </c>
@@ -2599,34 +3066,34 @@
         <v>212</v>
       </c>
       <c r="C39" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D39" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E39" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F39" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="G39" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="H39" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="I39" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="J39" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="K39" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="L39" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -2635,176 +3102,238 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="46.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.5703125" style="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" style="17" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="19.140625" style="17" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="15" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="2">
+    <row r="2" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="18">
         <v>2004</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="19" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="3">
+    <row r="3" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="20">
         <v>2005</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="21" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="2">
+    <row r="4" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="18">
         <v>2006</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="19" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="3">
+    <row r="5" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="20">
         <v>2007</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="21" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="2">
+    <row r="6" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="18">
         <v>2008</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="19" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="3">
+    <row r="7" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="20">
         <v>2009</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="21" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="2">
+    <row r="8" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="18">
         <v>2010</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+    </row>
+    <row r="9" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="20">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="18">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="20">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="18">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="20">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="18">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="20">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="18">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="20">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="18">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="20">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="20">
+        <v>2022</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2813,105 +3342,103 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.77734375" customWidth="1"/>
+    <col min="1" max="1" width="49.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="9"/>
-      <c r="B3" s="9" t="s">
+    <row r="3" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8" t="s">
+    <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="9"/>
-      <c r="B5" s="9" t="s">
+    <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="9" t="s">
+    <row r="6" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8" t="s">
+    <row r="7" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9" t="s">
+    <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8" t="s">
+    <row r="9" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9" t="s">
+    <row r="10" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="9" t="s">
+    <row r="11" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B11" s="9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="8" t="s">
+    </row>
+    <row r="13" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -2921,436 +3448,1309 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C44"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.77734375" customWidth="1"/>
-    <col min="2" max="2" width="40.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.7109375" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="106" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>318</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>181</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C6" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>182</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C7" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>108</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>110</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>111</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>112</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>183</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C13" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>184</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C14" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>226</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>113</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C16" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>114</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>224</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="C18" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>223</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>206</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="C21" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>115</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="11" t="s">
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>116</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>117</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>118</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>185</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C26" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>119</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="C1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>109</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>110</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>111</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>185</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="C5" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>186</v>
       </c>
-      <c r="B6" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="B28" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C28" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>112</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>113</v>
-      </c>
-      <c r="B8" s="11" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>187</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C29" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>188</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="C30" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>120</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>121</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>189</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="C33" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>122</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>190</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="C35" t="s">
+        <v>172</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>191</v>
+      </c>
+      <c r="B36" s="5" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>114</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>115</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>116</v>
-      </c>
-      <c r="B11" s="11" t="s">
+      <c r="C36" t="s">
+        <v>173</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>192</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="C37" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>193</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="C38" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>194</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="C39" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>123</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>283</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="C41" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>124</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>125</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>195</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C44" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>196</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="C45" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>197</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="C46" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>126</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>198</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="C48" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>127</v>
+      </c>
+      <c r="B49" s="5" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>187</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="C12" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>188</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="C13" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>117</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>142</v>
-      </c>
-      <c r="C14" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>118</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>67</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>119</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>120</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>121</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>122</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>189</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>145</v>
-      </c>
-      <c r="C21" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>123</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>190</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="C23" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>191</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="C24" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>192</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="C25" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>124</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>125</v>
-      </c>
-      <c r="B27" s="11" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>193</v>
-      </c>
-      <c r="B28" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="C28" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>126</v>
-      </c>
-      <c r="B29" s="11" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>194</v>
-      </c>
-      <c r="B30" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="C30" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>195</v>
-      </c>
-      <c r="B31" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="C31" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>196</v>
-      </c>
-      <c r="B32" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="C32" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>197</v>
-      </c>
-      <c r="B33" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="C33" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>198</v>
-      </c>
-      <c r="B34" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="C34" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>127</v>
-      </c>
-      <c r="B35" s="11" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>128</v>
-      </c>
-      <c r="B36" s="11" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>129</v>
-      </c>
-      <c r="B37" s="11" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>199</v>
       </c>
-      <c r="B38" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="C38" t="s">
+      <c r="B50" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="C50" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>200</v>
-      </c>
-      <c r="B39" s="11" t="s">
-        <v>160</v>
-      </c>
-      <c r="C39" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>201</v>
-      </c>
-      <c r="B40" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="C40" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>130</v>
-      </c>
-      <c r="B41" s="11" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>202</v>
-      </c>
-      <c r="B42" s="11" t="s">
-        <v>163</v>
-      </c>
-      <c r="C42" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>131</v>
-      </c>
-      <c r="B43" s="11" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>203</v>
-      </c>
-      <c r="B44" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="C44" t="s">
-        <v>184</v>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>309</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>310</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B64"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="63.7109375" style="28" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="101" style="29" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="27"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>229</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A3" s="28" t="s">
+        <v>305</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="28" t="s">
+        <v>130</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="28" t="s">
+        <v>261</v>
+      </c>
+      <c r="B5" s="29" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="28" t="s">
+        <v>232</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" s="28" t="s">
+        <v>304</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8" s="28" t="s">
+        <v>321</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="28" t="s">
+        <v>230</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="28" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="28" t="s">
+        <v>295</v>
+      </c>
+      <c r="B11" s="29" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="28" t="s">
+        <v>294</v>
+      </c>
+      <c r="B12" s="29" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="28" t="s">
+        <v>265</v>
+      </c>
+      <c r="B13" s="29" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="28" t="s">
+        <v>263</v>
+      </c>
+      <c r="B14" s="29" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="28" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="28" t="s">
+        <v>300</v>
+      </c>
+      <c r="B16" s="29" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="B17" s="29" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="28" t="s">
+        <v>233</v>
+      </c>
+      <c r="B18" s="29" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="B19" s="29" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A22" s="28" t="s">
+        <v>236</v>
+      </c>
+      <c r="B22" s="29" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A23" s="28" t="s">
+        <v>240</v>
+      </c>
+      <c r="B23" s="29" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="28" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="28" t="s">
+        <v>315</v>
+      </c>
+      <c r="B25" s="29" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="28" t="s">
+        <v>267</v>
+      </c>
+      <c r="B26" s="29" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="28" t="s">
+        <v>270</v>
+      </c>
+      <c r="B27" s="29" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="28" t="s">
+        <v>238</v>
+      </c>
+      <c r="B28" s="29" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" s="28" t="s">
+        <v>225</v>
+      </c>
+      <c r="B29" s="29" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A30" s="28" t="s">
+        <v>241</v>
+      </c>
+      <c r="B30" s="29" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A31" s="28" t="s">
+        <v>243</v>
+      </c>
+      <c r="B31" s="29" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="28" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="30"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="28" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="B35" s="29" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="28" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="28" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="28" t="s">
+        <v>316</v>
+      </c>
+      <c r="B38" s="29" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="28" t="s">
+        <v>277</v>
+      </c>
+      <c r="B39" s="29" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="28" t="s">
+        <v>279</v>
+      </c>
+      <c r="B40" s="29" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A41" s="23" t="s">
+        <v>253</v>
+      </c>
+      <c r="B41" s="24" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="28" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" s="30" t="s">
+        <v>255</v>
+      </c>
+      <c r="B47" s="29" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="B49" s="29" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A50" s="28" t="s">
+        <v>246</v>
+      </c>
+      <c r="B50" s="29" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" s="28" t="s">
+        <v>291</v>
+      </c>
+      <c r="B51" s="29" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A52" s="28" t="s">
+        <v>290</v>
+      </c>
+      <c r="B52" s="29" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A53" s="28" t="s">
+        <v>298</v>
+      </c>
+      <c r="B53" s="29" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A54" s="32" t="s">
+        <v>285</v>
+      </c>
+      <c r="B54" s="31" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A55" s="28" t="s">
+        <v>281</v>
+      </c>
+      <c r="B55" s="29" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="27"/>
+    </row>
+    <row r="57" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A57" s="32" t="s">
+        <v>248</v>
+      </c>
+      <c r="B57" s="31" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="32" t="s">
+        <v>256</v>
+      </c>
+      <c r="B58" s="31"/>
+    </row>
+    <row r="59" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A59" s="32" t="s">
+        <v>276</v>
+      </c>
+      <c r="B59" s="31" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A60" s="32" t="s">
+        <v>303</v>
+      </c>
+      <c r="B60" s="31" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A61" s="32" t="s">
+        <v>249</v>
+      </c>
+      <c r="B61" s="31" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A62" s="32" t="s">
+        <v>251</v>
+      </c>
+      <c r="B62" s="31" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A63" s="28" t="s">
+        <v>308</v>
+      </c>
+      <c r="B63" s="29" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A64" s="28" t="s">
+        <v>311</v>
+      </c>
+      <c r="B64" s="29" t="s">
+        <v>312</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="42.140625" customWidth="1"/>
+    <col min="3" max="3" width="68" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="8">
+        <v>44964</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="11"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
+        <v>44946</v>
+      </c>
+      <c r="B4" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
+        <v>44960</v>
+      </c>
+      <c r="B5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C5" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>213</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>216</v>
+      </c>
+      <c r="C7" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>44964</v>
+      </c>
+      <c r="B9" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>273</v>
+      </c>
+      <c r="C10" t="s">
+        <v>274</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010004CC22EA39550E4A8726E6152AFC908D" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="78e1b182962a7895ff8d998e3432f1d0">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="be6b2f93-bc73-451d-b641-99e8937f36fc" xmlns:ns4="1ac07a94-9fb2-4e93-a932-a54be51836dc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="526bf73398c13c38c503bb894a242dc1" ns3:_="" ns4:_="">
+    <xsd:import namespace="be6b2f93-bc73-451d-b641-99e8937f36fc"/>
+    <xsd:import namespace="1ac07a94-9fb2-4e93-a932-a54be51836dc"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns3:SharingHintHash" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceDateTaken" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="be6b2f93-bc73-451d-b641-99e8937f36fc" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="8" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="9" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="SharingHintHash" ma:index="10" nillable="true" ma:displayName="Sharing Hint Hash" ma:hidden="true" ma:internalName="SharingHintHash" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="1ac07a94-9fb2-4e93-a932-a54be51836dc" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="11" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="12" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="13" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="14" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="15" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="16" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="17" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA3F6F5D-FBC2-4FE9-A608-D5D7A6214624}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="1ac07a94-9fb2-4e93-a932-a54be51836dc"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be6b2f93-bc73-451d-b641-99e8937f36fc"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81DB2FF6-50F1-479E-A0AB-015E18BB6E14}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="be6b2f93-bc73-451d-b641-99e8937f36fc"/>
+    <ds:schemaRef ds:uri="1ac07a94-9fb2-4e93-a932-a54be51836dc"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7899FEF2-299D-45A9-8374-17448E3B5FA1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>